<commit_message>
. change sensor to blocks of device ids + add name filtering . refine filtering + add device_class
</commit_message>
<xml_diff>
--- a/components/bthome/_bthome_v1.xlsx
+++ b/components/bthome/_bthome_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Develop\Arduino\@esphome\esphome_components\bthome\components\bthome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2A3B882-E697-4B0C-8F10-7BEE08274031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378D8C4A-B1A4-4073-AC46-9239EF7BCB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12825" xr2:uid="{0A7624A3-1B95-4732-9BD7-3FA24DFCB5DE}"/>
   </bookViews>
@@ -16,10 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
   <si>
     <t>bject id</t>
   </si>
@@ -646,6 +645,57 @@
   </si>
   <si>
     <t>sensor.py - accuracy</t>
+  </si>
+  <si>
+    <t>device_class</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_BATTERY</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_TEMPERATURE</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_HUMIDITY</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_PRESSURE</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_ILLUMINANCE</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_ENERGY</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_POWER</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_VOLTAGE</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_PM10</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_MOISTURE</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_EMPTY</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_PM25</t>
+  </si>
+  <si>
+    <t>moisture2</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_CARBON_DIOXIDE</t>
+  </si>
+  <si>
+    <t>DEVICE_CLASS_VOLATILE_ORGANIC_COMPOUNDS</t>
   </si>
 </sst>
 </file>
@@ -690,10 +740,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1009,10 +1060,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{939659DA-A1AE-4233-819E-CB268DB45EEC}">
-  <dimension ref="A1:N67"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,15 +1077,17 @@
     <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" customWidth="1"/>
-    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" customWidth="1"/>
-    <col min="14" max="14" width="62.28515625" customWidth="1"/>
+    <col min="9" max="9" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25" customWidth="1"/>
+    <col min="15" max="15" width="23.28515625" customWidth="1"/>
+    <col min="16" max="16" width="62.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>180</v>
       </c>
@@ -1059,25 +1113,31 @@
         <v>5</v>
       </c>
       <c r="I1" t="s">
+        <v>202</v>
+      </c>
+      <c r="J1" t="s">
+        <v>203</v>
+      </c>
+      <c r="K1" t="s">
         <v>187</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>191</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>188</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>190</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>189</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <f t="shared" ref="A2:A49" si="0">HEX2DEC(SUBSTITUTE(B2,"0x",""))</f>
         <v>0</v>
@@ -1100,27 +1160,30 @@
       <c r="G2">
         <v>9</v>
       </c>
-      <c r="I2">
+      <c r="I2" t="s">
+        <v>214</v>
+      </c>
+      <c r="K2">
         <f>ABS(LOG10(E2))</f>
         <v>0</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>194</v>
       </c>
-      <c r="L2" t="str">
+      <c r="N2" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C2," ","_"),".","_"),"(",""),")","")</f>
         <v>packet_id</v>
       </c>
-      <c r="M2" t="str">
-        <f>"    """&amp;L2&amp;""": " &amp; B2 &amp; ","</f>
+      <c r="O2" t="str">
+        <f>"    """&amp;N2&amp;""": " &amp; B2 &amp; ","</f>
         <v xml:space="preserve">    "packet_id": 0x00,</v>
       </c>
-      <c r="N2" t="str">
-        <f>"    """&amp;L2&amp;""": {""measurement_type"": " &amp; B2 &amp; ", ""accuracy_decimals"": "&amp;I2&amp;", ""unit_of_measurement"":"""&amp;H2&amp;"""},"</f>
-        <v xml:space="preserve">    "packet_id": {"measurement_type": 0x00, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P2" s="3" t="str">
+        <f>"    """&amp;N2&amp;""": {""measurement_type"": " &amp; B2 &amp; ", ""accuracy_decimals"": "&amp;K2&amp;", ""unit_of_measurement"":"""&amp;H2&amp;""" , ""device_class"": "&amp;I2&amp;"},"</f>
+        <v xml:space="preserve">    "packet_id": {"measurement_type": 0x00, "accuracy_decimals": 0, "unit_of_measurement":"" , "device_class": DEVICE_CLASS_EMPTY},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1146,27 +1209,30 @@
       <c r="H3" t="s">
         <v>8</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I43" si="1">ABS(LOG10(E3))</f>
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="I3" t="s">
+        <v>204</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K43" si="1">ABS(LOG10(E3))</f>
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
         <v>194</v>
       </c>
-      <c r="L3" t="str">
-        <f t="shared" ref="L3:L49" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C3," ","_"),".","_"),"(",""),")","")</f>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N49" si="2">SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(C3," ","_"),".","_"),"(",""),")","")</f>
         <v>battery</v>
       </c>
-      <c r="M3" t="str">
-        <f t="shared" ref="M3:M49" si="3">"    """&amp;L3&amp;""": " &amp; B3 &amp; ","</f>
+      <c r="O3" t="str">
+        <f t="shared" ref="O3:O49" si="3">"    """&amp;N3&amp;""": " &amp; B3 &amp; ","</f>
         <v xml:space="preserve">    "battery": 0x01,</v>
       </c>
-      <c r="N3" t="str">
-        <f t="shared" ref="N3:N16" si="4">"    """&amp;L3&amp;""": {""measurement_type"": " &amp; B3 &amp; ", ""accuracy_decimals"": "&amp;I3&amp;", ""unit_of_measurement"":"""&amp;H3&amp;"""},"</f>
-        <v xml:space="preserve">    "battery": {"measurement_type": 0x01, "accuracy_decimals": 0, "unit_of_measurement":"%"},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P3" s="3" t="str">
+        <f t="shared" ref="P3:P16" si="4">"    """&amp;N3&amp;""": {""measurement_type"": " &amp; B3 &amp; ", ""accuracy_decimals"": "&amp;K3&amp;", ""unit_of_measurement"":"""&amp;H3&amp;""" , ""device_class"": "&amp;I3&amp;"},"</f>
+        <v xml:space="preserve">    "battery": {"measurement_type": 0x01, "accuracy_decimals": 0, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_BATTERY},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1192,31 +1258,34 @@
       <c r="H4" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="I4" t="s">
+        <v>205</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>194</v>
       </c>
-      <c r="K4" t="str">
-        <f t="shared" ref="K4:K10" si="5">" || obj_meas_type == "&amp;B4</f>
+      <c r="M4" t="str">
+        <f t="shared" ref="M4:M10" si="5">" || obj_meas_type == "&amp;B4</f>
         <v xml:space="preserve"> || obj_meas_type == 0x02</v>
       </c>
-      <c r="L4" t="str">
+      <c r="N4" t="str">
         <f t="shared" si="2"/>
         <v>temperature</v>
       </c>
-      <c r="M4" t="str">
+      <c r="O4" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "temperature": 0x02,</v>
       </c>
-      <c r="N4" t="str">
+      <c r="P4" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "temperature": {"measurement_type": 0x02, "accuracy_decimals": 2, "unit_of_measurement":"°C"},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "temperature": {"measurement_type": 0x02, "accuracy_decimals": 2, "unit_of_measurement":"°C" , "device_class": DEVICE_CLASS_TEMPERATURE},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1242,31 +1311,34 @@
       <c r="H5" t="s">
         <v>8</v>
       </c>
-      <c r="I5">
+      <c r="I5" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>194</v>
       </c>
-      <c r="K5" t="str">
+      <c r="M5" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> || obj_meas_type == 0x03</v>
       </c>
-      <c r="L5" t="str">
+      <c r="N5" t="str">
         <f t="shared" si="2"/>
         <v>humidity</v>
       </c>
-      <c r="M5" t="str">
+      <c r="O5" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "humidity": 0x03,</v>
       </c>
-      <c r="N5" t="str">
+      <c r="P5" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "humidity": {"measurement_type": 0x03, "accuracy_decimals": 2, "unit_of_measurement":"%"},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "humidity": {"measurement_type": 0x03, "accuracy_decimals": 2, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_HUMIDITY},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1292,31 +1364,34 @@
       <c r="H6" t="s">
         <v>20</v>
       </c>
-      <c r="I6">
+      <c r="I6" t="s">
+        <v>207</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>194</v>
       </c>
-      <c r="K6" t="str">
+      <c r="M6" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> || obj_meas_type == 0x04</v>
       </c>
-      <c r="L6" t="str">
+      <c r="N6" t="str">
         <f t="shared" si="2"/>
         <v>pressure</v>
       </c>
-      <c r="M6" t="str">
+      <c r="O6" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "pressure": 0x04,</v>
       </c>
-      <c r="N6" t="str">
+      <c r="P6" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "pressure": {"measurement_type": 0x04, "accuracy_decimals": 2, "unit_of_measurement":"hPa"},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "pressure": {"measurement_type": 0x04, "accuracy_decimals": 2, "unit_of_measurement":"hPa" , "device_class": DEVICE_CLASS_PRESSURE},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1342,31 +1417,34 @@
       <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="I7">
+      <c r="I7" t="s">
+        <v>208</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>194</v>
       </c>
-      <c r="K7" t="str">
+      <c r="M7" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> || obj_meas_type == 0x05</v>
       </c>
-      <c r="L7" t="str">
+      <c r="N7" t="str">
         <f t="shared" si="2"/>
         <v>illuminance</v>
       </c>
-      <c r="M7" t="str">
+      <c r="O7" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "illuminance": 0x05,</v>
       </c>
-      <c r="N7" t="str">
+      <c r="P7" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "illuminance": {"measurement_type": 0x05, "accuracy_decimals": 2, "unit_of_measurement":"lux"},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "illuminance": {"measurement_type": 0x05, "accuracy_decimals": 2, "unit_of_measurement":"lux" , "device_class": DEVICE_CLASS_ILLUMINANCE},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1392,31 +1470,34 @@
       <c r="H8" t="s">
         <v>28</v>
       </c>
-      <c r="I8">
+      <c r="I8" t="s">
+        <v>214</v>
+      </c>
+      <c r="K8">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L8" t="s">
         <v>194</v>
       </c>
-      <c r="K8" t="str">
+      <c r="M8" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> || obj_meas_type == 0x06</v>
       </c>
-      <c r="L8" t="str">
+      <c r="N8" t="str">
         <f t="shared" si="2"/>
         <v>mass_kg</v>
       </c>
-      <c r="M8" t="str">
+      <c r="O8" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "mass_kg": 0x06,</v>
       </c>
-      <c r="N8" t="str">
+      <c r="P8" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "mass_kg": {"measurement_type": 0x06, "accuracy_decimals": 2, "unit_of_measurement":"kg"},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "mass_kg": {"measurement_type": 0x06, "accuracy_decimals": 2, "unit_of_measurement":"kg" , "device_class": DEVICE_CLASS_EMPTY},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1442,31 +1523,34 @@
       <c r="H9" t="s">
         <v>32</v>
       </c>
-      <c r="I9">
+      <c r="I9" t="s">
+        <v>214</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
         <v>194</v>
       </c>
-      <c r="K9" t="str">
+      <c r="M9" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> || obj_meas_type == 0x07</v>
       </c>
-      <c r="L9" t="str">
+      <c r="N9" t="str">
         <f t="shared" si="2"/>
         <v>mass_lb</v>
       </c>
-      <c r="M9" t="str">
+      <c r="O9" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "mass_lb": 0x07,</v>
       </c>
-      <c r="N9" t="str">
+      <c r="P9" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "mass_lb": {"measurement_type": 0x07, "accuracy_decimals": 2, "unit_of_measurement":"lb"},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "mass_lb": {"measurement_type": 0x07, "accuracy_decimals": 2, "unit_of_measurement":"lb" , "device_class": DEVICE_CLASS_EMPTY},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1492,31 +1576,34 @@
       <c r="H10" t="s">
         <v>12</v>
       </c>
-      <c r="I10">
+      <c r="I10" t="s">
+        <v>214</v>
+      </c>
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>194</v>
       </c>
-      <c r="K10" t="str">
+      <c r="M10" t="str">
         <f t="shared" si="5"/>
         <v xml:space="preserve"> || obj_meas_type == 0x08</v>
       </c>
-      <c r="L10" t="str">
+      <c r="N10" t="str">
         <f t="shared" si="2"/>
         <v>dewpoint</v>
       </c>
-      <c r="M10" t="str">
+      <c r="O10" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "dewpoint": 0x08,</v>
       </c>
-      <c r="N10" t="str">
+      <c r="P10" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "dewpoint": {"measurement_type": 0x08, "accuracy_decimals": 2, "unit_of_measurement":"°C"},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "dewpoint": {"measurement_type": 0x08, "accuracy_decimals": 2, "unit_of_measurement":"°C" , "device_class": DEVICE_CLASS_EMPTY},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1539,27 +1626,30 @@
       <c r="G11">
         <v>96</v>
       </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="I11" t="s">
+        <v>214</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" t="s">
         <v>194</v>
       </c>
-      <c r="L11" t="str">
+      <c r="N11" t="str">
         <f t="shared" si="2"/>
         <v>count</v>
       </c>
-      <c r="M11" t="str">
+      <c r="O11" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "count": 0x09,</v>
       </c>
-      <c r="N11" t="str">
+      <c r="P11" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "count": {"measurement_type": 0x09, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "count": {"measurement_type": 0x09, "accuracy_decimals": 0, "unit_of_measurement":"" , "device_class": DEVICE_CLASS_EMPTY},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1585,31 +1675,34 @@
       <c r="H12" t="s">
         <v>40</v>
       </c>
-      <c r="I12">
+      <c r="I12" t="s">
+        <v>209</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>194</v>
       </c>
-      <c r="K12" t="str">
+      <c r="M12" t="str">
         <f>" || obj_meas_type == "&amp;B12</f>
         <v xml:space="preserve"> || obj_meas_type == 0x0A</v>
       </c>
-      <c r="L12" t="str">
+      <c r="N12" t="str">
         <f t="shared" si="2"/>
         <v>energy</v>
       </c>
-      <c r="M12" t="str">
+      <c r="O12" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "energy": 0x0A,</v>
       </c>
-      <c r="N12" t="str">
+      <c r="P12" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "energy": {"measurement_type": 0x0A, "accuracy_decimals": 3, "unit_of_measurement":"kWh"},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "energy": {"measurement_type": 0x0A, "accuracy_decimals": 3, "unit_of_measurement":"kWh" , "device_class": DEVICE_CLASS_ENERGY},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1635,31 +1728,34 @@
       <c r="H13" t="s">
         <v>44</v>
       </c>
-      <c r="I13">
+      <c r="I13" t="s">
+        <v>210</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>194</v>
       </c>
-      <c r="K13" t="str">
+      <c r="M13" t="str">
         <f>" || obj_meas_type == "&amp;B13</f>
         <v xml:space="preserve"> || obj_meas_type == 0x0B</v>
       </c>
-      <c r="L13" t="str">
+      <c r="N13" t="str">
         <f t="shared" si="2"/>
         <v>power</v>
       </c>
-      <c r="M13" t="str">
+      <c r="O13" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "power": 0x0B,</v>
       </c>
-      <c r="N13" t="str">
+      <c r="P13" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "power": {"measurement_type": 0x0B, "accuracy_decimals": 2, "unit_of_measurement":"W"},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "power": {"measurement_type": 0x0B, "accuracy_decimals": 2, "unit_of_measurement":"W" , "device_class": DEVICE_CLASS_POWER},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1685,31 +1781,34 @@
       <c r="H14" t="s">
         <v>48</v>
       </c>
-      <c r="I14">
+      <c r="I14" t="s">
+        <v>211</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>194</v>
       </c>
-      <c r="K14" t="str">
+      <c r="M14" t="str">
         <f>" || obj_meas_type == "&amp;B14</f>
         <v xml:space="preserve"> || obj_meas_type == 0x0C</v>
       </c>
-      <c r="L14" t="str">
+      <c r="N14" t="str">
         <f t="shared" si="2"/>
         <v>voltage</v>
       </c>
-      <c r="M14" t="str">
+      <c r="O14" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "voltage": 0x0C,</v>
       </c>
-      <c r="N14" t="str">
+      <c r="P14" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "voltage": {"measurement_type": 0x0C, "accuracy_decimals": 3, "unit_of_measurement":"V"},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "voltage": {"measurement_type": 0x0C, "accuracy_decimals": 3, "unit_of_measurement":"V" , "device_class": DEVICE_CLASS_VOLTAGE},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1735,27 +1834,30 @@
       <c r="H15" t="s">
         <v>52</v>
       </c>
-      <c r="I15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="I15" t="s">
+        <v>215</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L15" t="s">
         <v>194</v>
       </c>
-      <c r="L15" t="str">
+      <c r="N15" t="str">
         <f t="shared" si="2"/>
         <v>pm2_5</v>
       </c>
-      <c r="M15" t="str">
+      <c r="O15" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "pm2_5": 0x0D,</v>
       </c>
-      <c r="N15" t="str">
+      <c r="P15" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "pm2_5": {"measurement_type": 0x0D, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3"},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "pm2_5": {"measurement_type": 0x0D, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3" , "device_class": DEVICE_CLASS_PM25},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1781,27 +1883,30 @@
       <c r="H16" t="s">
         <v>52</v>
       </c>
-      <c r="I16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="I16" t="s">
+        <v>212</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L16" t="s">
         <v>194</v>
       </c>
-      <c r="L16" t="str">
+      <c r="N16" t="str">
         <f t="shared" si="2"/>
         <v>pm10</v>
       </c>
-      <c r="M16" t="str">
+      <c r="O16" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "pm10": 0x0E,</v>
       </c>
-      <c r="N16" t="str">
+      <c r="P16" s="3" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">    "pm10": {"measurement_type": 0x0E, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3"},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "pm10": {"measurement_type": 0x0E, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3" , "device_class": DEVICE_CLASS_PM10},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1824,23 +1929,27 @@
       <c r="G17" t="s">
         <v>70</v>
       </c>
-      <c r="I17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" t="s">
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L17" t="s">
         <v>192</v>
       </c>
-      <c r="L17" t="str">
+      <c r="N17" t="str">
         <f t="shared" si="2"/>
         <v>generic_boolean</v>
       </c>
-      <c r="M17" t="str">
+      <c r="O17" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "generic_boolean": 0x0F,</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P17" t="str">
+        <f t="shared" ref="P3:P49" si="6">"    """&amp;N17&amp;""": {""measurement_type"": " &amp; B17 &amp; ", ""accuracy_decimals"": "&amp;K17&amp;", ""unit_of_measurement"":"""&amp;H17&amp;"""},"</f>
+        <v xml:space="preserve">    "generic_boolean": {"measurement_type": 0x0F, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1863,23 +1972,27 @@
       <c r="G18" t="s">
         <v>70</v>
       </c>
-      <c r="I18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J18" t="s">
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L18" t="s">
         <v>192</v>
       </c>
-      <c r="L18" t="str">
+      <c r="N18" t="str">
         <f t="shared" si="2"/>
         <v>power</v>
       </c>
-      <c r="M18" t="str">
+      <c r="O18" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "power": 0x10,</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P18" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "power": {"measurement_type": 0x10, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1902,23 +2015,27 @@
       <c r="G19" t="s">
         <v>74</v>
       </c>
-      <c r="I19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J19" t="s">
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L19" t="s">
         <v>192</v>
       </c>
-      <c r="L19" t="str">
+      <c r="N19" t="str">
         <f t="shared" si="2"/>
         <v>opening</v>
       </c>
-      <c r="M19" t="str">
+      <c r="O19" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "opening": 0x11,</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P19" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "opening": {"measurement_type": 0x11, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1944,27 +2061,30 @@
       <c r="H20" t="s">
         <v>58</v>
       </c>
-      <c r="I20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20" t="s">
+      <c r="I20" t="s">
+        <v>217</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L20" t="s">
         <v>194</v>
       </c>
-      <c r="L20" t="str">
+      <c r="N20" t="str">
         <f t="shared" si="2"/>
         <v>co2</v>
       </c>
-      <c r="M20" t="str">
+      <c r="O20" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "co2": 0x12,</v>
       </c>
-      <c r="N20" t="str">
-        <f>"    """&amp;L20&amp;""": {""measurement_type"": " &amp; B20 &amp; ", ""accuracy_decimals"": "&amp;I20&amp;", ""unit_of_measurement"":"""&amp;H20&amp;"""},"</f>
-        <v xml:space="preserve">    "co2": {"measurement_type": 0x12, "accuracy_decimals": 0, "unit_of_measurement":"ppm"},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P20" s="3" t="str">
+        <f t="shared" ref="P20:P22" si="7">"    """&amp;N20&amp;""": {""measurement_type"": " &amp; B20 &amp; ", ""accuracy_decimals"": "&amp;K20&amp;", ""unit_of_measurement"":"""&amp;H20&amp;""" , ""device_class"": "&amp;I20&amp;"},"</f>
+        <v xml:space="preserve">    "co2": {"measurement_type": 0x12, "accuracy_decimals": 0, "unit_of_measurement":"ppm" , "device_class": DEVICE_CLASS_CARBON_DIOXIDE},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1990,27 +2110,30 @@
       <c r="H21" t="s">
         <v>52</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="I21" t="s">
+        <v>218</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L21" t="s">
         <v>194</v>
       </c>
-      <c r="L21" t="str">
+      <c r="N21" t="str">
         <f t="shared" si="2"/>
         <v>tvoc</v>
       </c>
-      <c r="M21" t="str">
+      <c r="O21" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "tvoc": 0x13,</v>
       </c>
-      <c r="N21" t="str">
-        <f>"    """&amp;L21&amp;""": {""measurement_type"": " &amp; B21 &amp; ", ""accuracy_decimals"": "&amp;I21&amp;", ""unit_of_measurement"":"""&amp;H21&amp;"""},"</f>
-        <v xml:space="preserve">    "tvoc": {"measurement_type": 0x13, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3"},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P21" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">    "tvoc": {"measurement_type": 0x13, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3" , "device_class": DEVICE_CLASS_VOLATILE_ORGANIC_COMPOUNDS},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2036,31 +2159,34 @@
       <c r="H22" t="s">
         <v>8</v>
       </c>
-      <c r="I22">
+      <c r="I22" t="s">
+        <v>213</v>
+      </c>
+      <c r="K22">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="J22" t="s">
+      <c r="L22" t="s">
         <v>194</v>
       </c>
-      <c r="K22" t="str">
+      <c r="M22" t="str">
         <f>" || obj_meas_type == "&amp;B22</f>
         <v xml:space="preserve"> || obj_meas_type == 0x14</v>
       </c>
-      <c r="L22" t="str">
+      <c r="N22" t="str">
         <f t="shared" si="2"/>
         <v>moisture</v>
       </c>
-      <c r="M22" t="str">
+      <c r="O22" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "moisture": 0x14,</v>
       </c>
-      <c r="N22" t="str">
-        <f>"    """&amp;L22&amp;""": {""measurement_type"": " &amp; B22 &amp; ", ""accuracy_decimals"": "&amp;I22&amp;", ""unit_of_measurement"":"""&amp;H22&amp;"""},"</f>
-        <v xml:space="preserve">    "moisture": {"measurement_type": 0x14, "accuracy_decimals": 2, "unit_of_measurement":"%"},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P22" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v xml:space="preserve">    "moisture": {"measurement_type": 0x14, "accuracy_decimals": 2, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_MOISTURE},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2083,23 +2209,27 @@
       <c r="G23" t="s">
         <v>76</v>
       </c>
-      <c r="I23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J23" t="s">
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L23" t="s">
         <v>192</v>
       </c>
-      <c r="L23" t="str">
+      <c r="N23" t="str">
         <f t="shared" si="2"/>
         <v>battery</v>
       </c>
-      <c r="M23" t="str">
+      <c r="O23" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "battery": 0x15,</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P23" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "battery": {"measurement_type": 0x15, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2122,23 +2252,27 @@
       <c r="G24" t="s">
         <v>79</v>
       </c>
-      <c r="I24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24" t="s">
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L24" t="s">
         <v>192</v>
       </c>
-      <c r="L24" t="str">
+      <c r="N24" t="str">
         <f t="shared" si="2"/>
         <v>battery_charging</v>
       </c>
-      <c r="M24" t="str">
+      <c r="O24" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "battery_charging": 0x16,</v>
       </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P24" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "battery_charging": {"measurement_type": 0x16, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2161,23 +2295,27 @@
       <c r="G25" t="s">
         <v>82</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J25" t="s">
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
         <v>192</v>
       </c>
-      <c r="L25" t="str">
+      <c r="N25" t="str">
         <f t="shared" si="2"/>
         <v>carbon_monoxide</v>
       </c>
-      <c r="M25" t="str">
+      <c r="O25" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "carbon_monoxide": 0x17,</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P25" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "carbon_monoxide": {"measurement_type": 0x17, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2200,23 +2338,27 @@
       <c r="G26" t="s">
         <v>85</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="K26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L26" t="s">
         <v>192</v>
       </c>
-      <c r="L26" t="str">
+      <c r="N26" t="str">
         <f t="shared" si="2"/>
         <v>cold</v>
       </c>
-      <c r="M26" t="str">
+      <c r="O26" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "cold": 0x18,</v>
       </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P26" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "cold": {"measurement_type": 0x18, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2239,23 +2381,27 @@
       <c r="G27" t="s">
         <v>88</v>
       </c>
-      <c r="I27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L27" t="s">
         <v>192</v>
       </c>
-      <c r="L27" t="str">
+      <c r="N27" t="str">
         <f t="shared" si="2"/>
         <v>connectivity</v>
       </c>
-      <c r="M27" t="str">
+      <c r="O27" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "connectivity": 0x19,</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P27" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "connectivity": {"measurement_type": 0x19, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2278,23 +2424,27 @@
       <c r="G28" t="s">
         <v>74</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
         <v>192</v>
       </c>
-      <c r="L28" t="str">
+      <c r="N28" t="str">
         <f t="shared" si="2"/>
         <v>door</v>
       </c>
-      <c r="M28" t="str">
+      <c r="O28" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "door": 0x1A,</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P28" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "door": {"measurement_type": 0x1A, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2317,23 +2467,27 @@
       <c r="G29" t="s">
         <v>74</v>
       </c>
-      <c r="I29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
         <v>192</v>
       </c>
-      <c r="L29" t="str">
+      <c r="N29" t="str">
         <f t="shared" si="2"/>
         <v>garage_door</v>
       </c>
-      <c r="M29" t="str">
+      <c r="O29" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "garage_door": 0x1B,</v>
       </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P29" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "garage_door": {"measurement_type": 0x1B, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2356,23 +2510,27 @@
       <c r="G30" t="s">
         <v>98</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J30" t="s">
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L30" t="s">
         <v>192</v>
       </c>
-      <c r="L30" t="str">
+      <c r="N30" t="str">
         <f t="shared" si="2"/>
         <v>gas</v>
       </c>
-      <c r="M30" t="str">
+      <c r="O30" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "gas": 0x1C,</v>
       </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P30" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "gas": {"measurement_type": 0x1C, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2395,23 +2553,27 @@
       <c r="G31" t="s">
         <v>102</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J31" t="s">
+      <c r="K31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L31" t="s">
         <v>192</v>
       </c>
-      <c r="L31" t="str">
+      <c r="N31" t="str">
         <f t="shared" si="2"/>
         <v>heat</v>
       </c>
-      <c r="M31" t="str">
+      <c r="O31" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "heat": 0x1D,</v>
       </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P31" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "heat": {"measurement_type": 0x1D, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2434,23 +2596,27 @@
       <c r="G32" t="s">
         <v>105</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J32" t="s">
+      <c r="K32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L32" t="s">
         <v>192</v>
       </c>
-      <c r="L32" t="str">
+      <c r="N32" t="str">
         <f t="shared" si="2"/>
         <v>light</v>
       </c>
-      <c r="M32" t="str">
+      <c r="O32" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "light": 0x1E,</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P32" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "light": {"measurement_type": 0x1E, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2473,23 +2639,27 @@
       <c r="G33" t="s">
         <v>109</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J33" t="s">
+      <c r="K33">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L33" t="s">
         <v>192</v>
       </c>
-      <c r="L33" t="str">
+      <c r="N33" t="str">
         <f t="shared" si="2"/>
         <v>lock</v>
       </c>
-      <c r="M33" t="str">
+      <c r="O33" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "lock": 0x1F,</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P33" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "lock": {"measurement_type": 0x1F, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2512,23 +2682,27 @@
       <c r="G34" t="s">
         <v>111</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J34" t="s">
+      <c r="K34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L34" t="s">
         <v>192</v>
       </c>
-      <c r="L34" t="str">
+      <c r="N34" t="str">
         <f t="shared" si="2"/>
         <v>moisture</v>
       </c>
-      <c r="M34" t="str">
+      <c r="O34" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "moisture": 0x20,</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P34" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "moisture": {"measurement_type": 0x20, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2551,23 +2725,27 @@
       <c r="G35" t="s">
         <v>114</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="K35">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L35" t="s">
         <v>192</v>
       </c>
-      <c r="L35" t="str">
+      <c r="N35" t="str">
         <f t="shared" si="2"/>
         <v>motion</v>
       </c>
-      <c r="M35" t="str">
+      <c r="O35" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "motion": 0x21,</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P35" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "motion": {"measurement_type": 0x21, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2590,23 +2768,27 @@
       <c r="G36" t="s">
         <v>117</v>
       </c>
-      <c r="I36">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L36" t="s">
         <v>192</v>
       </c>
-      <c r="L36" t="str">
+      <c r="N36" t="str">
         <f t="shared" si="2"/>
         <v>moving</v>
       </c>
-      <c r="M36" t="str">
+      <c r="O36" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "moving": 0x22,</v>
       </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P36" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "moving": {"measurement_type": 0x22, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2629,23 +2811,27 @@
       <c r="G37" t="s">
         <v>98</v>
       </c>
-      <c r="I37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J37" t="s">
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L37" t="s">
         <v>192</v>
       </c>
-      <c r="L37" t="str">
+      <c r="N37" t="str">
         <f t="shared" si="2"/>
         <v>occupancy</v>
       </c>
-      <c r="M37" t="str">
+      <c r="O37" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "occupancy": 0x23,</v>
       </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P37" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "occupancy": {"measurement_type": 0x23, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2668,23 +2854,27 @@
       <c r="G38" t="s">
         <v>122</v>
       </c>
-      <c r="I38">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J38" t="s">
+      <c r="K38">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L38" t="s">
         <v>192</v>
       </c>
-      <c r="L38" t="str">
+      <c r="N38" t="str">
         <f t="shared" si="2"/>
         <v>plug</v>
       </c>
-      <c r="M38" t="str">
+      <c r="O38" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "plug": 0x24,</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P38" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "plug": {"measurement_type": 0x24, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2707,23 +2897,27 @@
       <c r="G39" t="s">
         <v>125</v>
       </c>
-      <c r="I39">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J39" t="s">
+      <c r="K39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L39" t="s">
         <v>192</v>
       </c>
-      <c r="L39" t="str">
+      <c r="N39" t="str">
         <f t="shared" si="2"/>
         <v>presence</v>
       </c>
-      <c r="M39" t="str">
+      <c r="O39" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "presence": 0x25,</v>
       </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P39" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "presence": {"measurement_type": 0x25, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2746,23 +2940,27 @@
       <c r="G40" t="s">
         <v>128</v>
       </c>
-      <c r="I40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J40" t="s">
+      <c r="K40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L40" t="s">
         <v>192</v>
       </c>
-      <c r="L40" t="str">
+      <c r="N40" t="str">
         <f t="shared" si="2"/>
         <v>problem</v>
       </c>
-      <c r="M40" t="str">
+      <c r="O40" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "problem": 0x26,</v>
       </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P40" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "problem": {"measurement_type": 0x26, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2785,23 +2983,27 @@
       <c r="G41" t="s">
         <v>131</v>
       </c>
-      <c r="I41">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J41" t="s">
+      <c r="K41">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L41" t="s">
         <v>192</v>
       </c>
-      <c r="L41" t="str">
+      <c r="N41" t="str">
         <f t="shared" si="2"/>
         <v>running</v>
       </c>
-      <c r="M41" t="str">
+      <c r="O41" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "running": 0x27,</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P41" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "running": {"measurement_type": 0x27, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2824,23 +3026,27 @@
       <c r="G42" t="s">
         <v>134</v>
       </c>
-      <c r="I42">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="K42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L42" t="s">
         <v>192</v>
       </c>
-      <c r="L42" t="str">
+      <c r="N42" t="str">
         <f t="shared" si="2"/>
         <v>safety</v>
       </c>
-      <c r="M42" t="str">
+      <c r="O42" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "safety": 0x28,</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P42" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "safety": {"measurement_type": 0x28, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2863,23 +3069,27 @@
       <c r="G43" t="s">
         <v>98</v>
       </c>
-      <c r="I43">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J43" t="s">
+      <c r="K43">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L43" t="s">
         <v>192</v>
       </c>
-      <c r="L43" t="str">
+      <c r="N43" t="str">
         <f t="shared" si="2"/>
         <v>smoke</v>
       </c>
-      <c r="M43" t="str">
+      <c r="O43" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "smoke": 0x29,</v>
       </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P43" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "smoke": {"measurement_type": 0x29, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2902,23 +3112,27 @@
       <c r="G44" t="s">
         <v>114</v>
       </c>
-      <c r="I44">
-        <f t="shared" ref="I44:I49" si="6">ABS(LOG10(E44))</f>
-        <v>0</v>
-      </c>
-      <c r="J44" t="s">
+      <c r="K44">
+        <f t="shared" ref="K44:K49" si="8">ABS(LOG10(E44))</f>
+        <v>0</v>
+      </c>
+      <c r="L44" t="s">
         <v>192</v>
       </c>
-      <c r="L44" t="str">
+      <c r="N44" t="str">
         <f t="shared" si="2"/>
         <v>sound</v>
       </c>
-      <c r="M44" t="str">
+      <c r="O44" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "sound": 0x2A,</v>
       </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P44" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">    "sound": {"measurement_type": 0x2A, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2941,23 +3155,27 @@
       <c r="G45" t="s">
         <v>143</v>
       </c>
-      <c r="I45">
+      <c r="K45">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L45" t="s">
+        <v>192</v>
+      </c>
+      <c r="N45" t="str">
+        <f t="shared" si="2"/>
+        <v>tamper</v>
+      </c>
+      <c r="O45" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "tamper": 0x2B,</v>
+      </c>
+      <c r="P45" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J45" t="s">
-        <v>192</v>
-      </c>
-      <c r="L45" t="str">
-        <f t="shared" si="2"/>
-        <v>tamper</v>
-      </c>
-      <c r="M45" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    "tamper": 0x2B,</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "tamper": {"measurement_type": 0x2B, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2980,23 +3198,27 @@
       <c r="G46" t="s">
         <v>98</v>
       </c>
-      <c r="I46">
+      <c r="K46">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L46" t="s">
+        <v>192</v>
+      </c>
+      <c r="N46" t="str">
+        <f t="shared" si="2"/>
+        <v>vibration</v>
+      </c>
+      <c r="O46" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "vibration": 0x2C,</v>
+      </c>
+      <c r="P46" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J46" t="s">
-        <v>192</v>
-      </c>
-      <c r="L46" t="str">
-        <f t="shared" si="2"/>
-        <v>vibration</v>
-      </c>
-      <c r="M46" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    "vibration": 0x2C,</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "vibration": {"measurement_type": 0x2C, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -3019,23 +3241,27 @@
       <c r="G47" t="s">
         <v>74</v>
       </c>
-      <c r="I47">
+      <c r="K47">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L47" t="s">
+        <v>192</v>
+      </c>
+      <c r="N47" t="str">
+        <f t="shared" si="2"/>
+        <v>window</v>
+      </c>
+      <c r="O47" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "window": 0x2D,</v>
+      </c>
+      <c r="P47" t="str">
         <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J47" t="s">
-        <v>192</v>
-      </c>
-      <c r="L47" t="str">
-        <f t="shared" si="2"/>
-        <v>window</v>
-      </c>
-      <c r="M47" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    "window": 0x2D,</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+        <v xml:space="preserve">    "window": {"measurement_type": 0x2D, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -3061,27 +3287,30 @@
       <c r="H48" t="s">
         <v>8</v>
       </c>
-      <c r="I48">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="I48" t="s">
+        <v>206</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L48" t="s">
         <v>194</v>
       </c>
-      <c r="L48" t="str">
+      <c r="N48" t="str">
         <f t="shared" si="2"/>
         <v>humidity2</v>
       </c>
-      <c r="M48" t="str">
+      <c r="O48" t="str">
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "humidity2": 0x2E,</v>
       </c>
-      <c r="N48" t="str">
-        <f>"    """&amp;L48&amp;""": {""measurement_type"": " &amp; B48 &amp; ", ""accuracy_decimals"": "&amp;I48&amp;", ""unit_of_measurement"":"""&amp;H48&amp;"""},"</f>
-        <v xml:space="preserve">    "humidity2": {"measurement_type": 0x2E, "accuracy_decimals": 0, "unit_of_measurement":"%"},</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P48" s="3" t="str">
+        <f t="shared" ref="P48:P49" si="9">"    """&amp;N48&amp;""": {""measurement_type"": " &amp; B48 &amp; ", ""accuracy_decimals"": "&amp;K48&amp;", ""unit_of_measurement"":"""&amp;H48&amp;""" , ""device_class"": "&amp;I48&amp;"},"</f>
+        <v xml:space="preserve">    "humidity2": {"measurement_type": 0x2E, "accuracy_decimals": 0, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_HUMIDITY},</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -3090,7 +3319,7 @@
         <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>62</v>
+        <v>216</v>
       </c>
       <c r="D49" t="s">
         <v>68</v>
@@ -3107,37 +3336,40 @@
       <c r="H49" t="s">
         <v>8</v>
       </c>
-      <c r="I49">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J49" t="s">
+      <c r="I49" t="s">
+        <v>213</v>
+      </c>
+      <c r="K49">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L49" t="s">
         <v>194</v>
       </c>
-      <c r="L49" t="str">
-        <f t="shared" si="2"/>
-        <v>moisture</v>
-      </c>
-      <c r="M49" t="str">
-        <f t="shared" si="3"/>
-        <v xml:space="preserve">    "moisture": 0x2F,</v>
-      </c>
       <c r="N49" t="str">
-        <f>"    """&amp;L49&amp;""": {""measurement_type"": " &amp; B49 &amp; ", ""accuracy_decimals"": "&amp;I49&amp;", ""unit_of_measurement"":"""&amp;H49&amp;"""},"</f>
-        <v xml:space="preserve">    "moisture": {"measurement_type": 0x2F, "accuracy_decimals": 0, "unit_of_measurement":"%"},</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>moisture2</v>
+      </c>
+      <c r="O49" t="str">
+        <f t="shared" si="3"/>
+        <v xml:space="preserve">    "moisture2": 0x2F,</v>
+      </c>
+      <c r="P49" s="3" t="str">
+        <f t="shared" si="9"/>
+        <v xml:space="preserve">    "moisture2": {"measurement_type": 0x2F, "accuracy_decimals": 0, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_MOISTURE},</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -3160,7 +3392,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>152</v>
       </c>
@@ -3177,7 +3409,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C59" t="s">
         <v>6</v>
       </c>
@@ -3191,7 +3423,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>9</v>
       </c>
@@ -3205,7 +3437,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>13</v>
       </c>
@@ -3219,7 +3451,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>17</v>
       </c>
@@ -3233,7 +3465,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C63" t="s">
         <v>21</v>
       </c>
@@ -3247,7 +3479,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C64" t="s">
         <v>25</v>
       </c>
@@ -3313,7 +3545,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M49" xr:uid="{939659DA-A1AE-4233-819E-CB268DB45EEC}"/>
+  <autoFilter ref="A1:O49" xr:uid="{939659DA-A1AE-4233-819E-CB268DB45EEC}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="nonbinary"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F39">
     <sortCondition ref="A2:A39"/>
   </sortState>

</xml_diff>

<commit_message>
initial add for BTHomeV2 parser
</commit_message>
<xml_diff>
--- a/components/bthome/_bthome_v1.xlsx
+++ b/components/bthome/_bthome_v1.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Develop\Arduino\@esphome\esphome_components\bthome\components\bthome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378D8C4A-B1A4-4073-AC46-9239EF7BCB34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CEB9D01-4086-4BEC-B369-627D1AA0450E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12825" xr2:uid="{0A7624A3-1B95-4732-9BD7-3FA24DFCB5DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="12825" activeTab="1" xr2:uid="{0A7624A3-1B95-4732-9BD7-3FA24DFCB5DE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="V1" sheetId="1" r:id="rId1"/>
+    <sheet name="V2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V1'!$A$1:$O$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'V2'!$A$1:$I$81</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="357">
   <si>
     <t>bject id</t>
   </si>
@@ -696,13 +698,429 @@
   </si>
   <si>
     <t>DEVICE_CLASS_VOLATILE_ORGANIC_COMPOUNDS</t>
+  </si>
+  <si>
+    <t>uint (1 bytes)</t>
+  </si>
+  <si>
+    <t>0x3D</t>
+  </si>
+  <si>
+    <t>uint (2 bytes)</t>
+  </si>
+  <si>
+    <t>3D0960</t>
+  </si>
+  <si>
+    <t>0x3E</t>
+  </si>
+  <si>
+    <t>3E2A2C0960</t>
+  </si>
+  <si>
+    <t>0x43</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>08CA06</t>
+  </si>
+  <si>
+    <t>0x40</t>
+  </si>
+  <si>
+    <t>distance (mm)</t>
+  </si>
+  <si>
+    <t>400C00</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>0x41</t>
+  </si>
+  <si>
+    <t>distance (m)</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>0x42</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>424E3400</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>0x4D</t>
+  </si>
+  <si>
+    <t>uint32 (4 bytes)</t>
+  </si>
+  <si>
+    <t>4d12138a14</t>
+  </si>
+  <si>
+    <t>0A138A14</t>
+  </si>
+  <si>
+    <t>0x4B</t>
+  </si>
+  <si>
+    <t>4B138A14</t>
+  </si>
+  <si>
+    <t>m3</t>
+  </si>
+  <si>
+    <t>0x4C</t>
+  </si>
+  <si>
+    <t>4C41018A01</t>
+  </si>
+  <si>
+    <t>03BF13</t>
+  </si>
+  <si>
+    <t>05138A14</t>
+  </si>
+  <si>
+    <t>065E1F</t>
+  </si>
+  <si>
+    <t>073E1D</t>
+  </si>
+  <si>
+    <t>14020C</t>
+  </si>
+  <si>
+    <t>2F23</t>
+  </si>
+  <si>
+    <t>0D120C</t>
+  </si>
+  <si>
+    <t>0E021C</t>
+  </si>
+  <si>
+    <t>0B021B00</t>
+  </si>
+  <si>
+    <t>04138A01</t>
+  </si>
+  <si>
+    <t>0x3F</t>
+  </si>
+  <si>
+    <t>rotation</t>
+  </si>
+  <si>
+    <t>3F020C</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>0x44</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>m/s</t>
+  </si>
+  <si>
+    <t>0x45</t>
+  </si>
+  <si>
+    <t>02CA09</t>
+  </si>
+  <si>
+    <t>0C020C</t>
+  </si>
+  <si>
+    <t>0x4A</t>
+  </si>
+  <si>
+    <t>4A020C</t>
+  </si>
+  <si>
+    <t>0x4E</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>4E87562A01</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>0x47</t>
+  </si>
+  <si>
+    <t>0x48</t>
+  </si>
+  <si>
+    <t>48DC87</t>
+  </si>
+  <si>
+    <t>mL</t>
+  </si>
+  <si>
+    <t>0x49</t>
+  </si>
+  <si>
+    <t>volume Flow Rate</t>
+  </si>
+  <si>
+    <t>49DC87</t>
+  </si>
+  <si>
+    <t>m3/hr</t>
+  </si>
+  <si>
+    <t>0x46</t>
+  </si>
+  <si>
+    <t>UV index</t>
+  </si>
+  <si>
+    <t>0x4F</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>4F87562A01</t>
+  </si>
+  <si>
+    <t>0161</t>
+  </si>
+  <si>
+    <t>12E204</t>
+  </si>
+  <si>
+    <t>0960</t>
+  </si>
+  <si>
+    <t>434E34</t>
+  </si>
+  <si>
+    <t>414E00</t>
+  </si>
+  <si>
+    <t>2E23</t>
+  </si>
+  <si>
+    <t>444E34</t>
+  </si>
+  <si>
+    <t>451101</t>
+  </si>
+  <si>
+    <t>133301</t>
+  </si>
+  <si>
+    <t>478756</t>
+  </si>
+  <si>
+    <t>4632</t>
+  </si>
+  <si>
+    <t>1A00</t>
+  </si>
+  <si>
+    <t>1B01</t>
+  </si>
+  <si>
+    <t>1C01</t>
+  </si>
+  <si>
+    <t>0F01</t>
+  </si>
+  <si>
+    <t>1D00</t>
+  </si>
+  <si>
+    <t>1F01</t>
+  </si>
+  <si>
+    <t>2A00</t>
+  </si>
+  <si>
+    <t>2B00</t>
+  </si>
+  <si>
+    <t>2C01</t>
+  </si>
+  <si>
+    <t>2D01</t>
+  </si>
+  <si>
+    <t>0 (False = Normal), 1 (True = Low)</t>
+  </si>
+  <si>
+    <t>0 (False = Not Charging), 1 (True = Charging)</t>
+  </si>
+  <si>
+    <t>0 (False = Not detected), 1 (True = Detected)</t>
+  </si>
+  <si>
+    <t>0 (False = Normal), 1 (True = Cold)</t>
+  </si>
+  <si>
+    <t>0 (False = Disconnected), 1 (True = Connected)</t>
+  </si>
+  <si>
+    <t>0 (False = Closed), 1 (True = Open)</t>
+  </si>
+  <si>
+    <t>0 (False = Clear), 1 (True = Detected)</t>
+  </si>
+  <si>
+    <t>0 (False = Off), 1 (True = On)</t>
+  </si>
+  <si>
+    <t>0 (False = Normal), 1 (True = Hot)</t>
+  </si>
+  <si>
+    <t>0 (False = No light), 1 (True = Light detected)</t>
+  </si>
+  <si>
+    <t>0 (False = Locked), 1 (True = Unlocked)</t>
+  </si>
+  <si>
+    <t>0 (False = Dry), 1 (True = Wet)</t>
+  </si>
+  <si>
+    <t>0 (False = Not moving), 1 (True = Moving)</t>
+  </si>
+  <si>
+    <t>0 (False = Unplugged), 1 (True = Plugged in)</t>
+  </si>
+  <si>
+    <t>0 (False = Away), 1 (True = Home)</t>
+  </si>
+  <si>
+    <t>0 (False = OK), 1 (True = Problem)</t>
+  </si>
+  <si>
+    <t>0 (False = Not Running), 1 (True = Running)</t>
+  </si>
+  <si>
+    <t>0 (False = Unsafe), 1 (True = Safe)</t>
+  </si>
+  <si>
+    <t>3A00</t>
+  </si>
+  <si>
+    <t>3A01</t>
+  </si>
+  <si>
+    <t>3A02</t>
+  </si>
+  <si>
+    <t>3A03</t>
+  </si>
+  <si>
+    <t>3A04</t>
+  </si>
+  <si>
+    <t>3A05</t>
+  </si>
+  <si>
+    <t>3A06</t>
+  </si>
+  <si>
+    <t>3C00</t>
+  </si>
+  <si>
+    <t>3C0103</t>
+  </si>
+  <si>
+    <t>3C020A</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>objid_dec</t>
+  </si>
+  <si>
+    <t>0x30</t>
+  </si>
+  <si>
+    <t>0x31</t>
+  </si>
+  <si>
+    <t>0x32</t>
+  </si>
+  <si>
+    <t>0x33</t>
+  </si>
+  <si>
+    <t>0x34</t>
+  </si>
+  <si>
+    <t>0x35</t>
+  </si>
+  <si>
+    <t>0x36</t>
+  </si>
+  <si>
+    <t>0x37</t>
+  </si>
+  <si>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>0x39</t>
+  </si>
+  <si>
+    <t>0x3B</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>DataLen
+123</t>
+  </si>
+  <si>
+    <t>DataType
+45</t>
+  </si>
+  <si>
+    <t>TypeByte</t>
+  </si>
+  <si>
+    <t>TypeByteCommmented</t>
+  </si>
+  <si>
+    <t>Factor 67</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -714,6 +1132,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -740,11 +1166,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1063,8 +1499,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I52" sqref="I52"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1614,7 @@
         <f>"    """&amp;N2&amp;""": " &amp; B2 &amp; ","</f>
         <v xml:space="preserve">    "packet_id": 0x00,</v>
       </c>
-      <c r="P2" s="3" t="str">
+      <c r="P2" t="str">
         <f>"    """&amp;N2&amp;""": {""measurement_type"": " &amp; B2 &amp; ", ""accuracy_decimals"": "&amp;K2&amp;", ""unit_of_measurement"":"""&amp;H2&amp;""" , ""device_class"": "&amp;I2&amp;"},"</f>
         <v xml:space="preserve">    "packet_id": {"measurement_type": 0x00, "accuracy_decimals": 0, "unit_of_measurement":"" , "device_class": DEVICE_CLASS_EMPTY},</v>
       </c>
@@ -1227,7 +1663,7 @@
         <f t="shared" ref="O3:O49" si="3">"    """&amp;N3&amp;""": " &amp; B3 &amp; ","</f>
         <v xml:space="preserve">    "battery": 0x01,</v>
       </c>
-      <c r="P3" s="3" t="str">
+      <c r="P3" t="str">
         <f t="shared" ref="P3:P16" si="4">"    """&amp;N3&amp;""": {""measurement_type"": " &amp; B3 &amp; ", ""accuracy_decimals"": "&amp;K3&amp;", ""unit_of_measurement"":"""&amp;H3&amp;""" , ""device_class"": "&amp;I3&amp;"},"</f>
         <v xml:space="preserve">    "battery": {"measurement_type": 0x01, "accuracy_decimals": 0, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_BATTERY},</v>
       </c>
@@ -1280,7 +1716,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "temperature": 0x02,</v>
       </c>
-      <c r="P4" s="3" t="str">
+      <c r="P4" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "temperature": {"measurement_type": 0x02, "accuracy_decimals": 2, "unit_of_measurement":"°C" , "device_class": DEVICE_CLASS_TEMPERATURE},</v>
       </c>
@@ -1333,7 +1769,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "humidity": 0x03,</v>
       </c>
-      <c r="P5" s="3" t="str">
+      <c r="P5" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "humidity": {"measurement_type": 0x03, "accuracy_decimals": 2, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_HUMIDITY},</v>
       </c>
@@ -1386,7 +1822,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "pressure": 0x04,</v>
       </c>
-      <c r="P6" s="3" t="str">
+      <c r="P6" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "pressure": {"measurement_type": 0x04, "accuracy_decimals": 2, "unit_of_measurement":"hPa" , "device_class": DEVICE_CLASS_PRESSURE},</v>
       </c>
@@ -1439,7 +1875,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "illuminance": 0x05,</v>
       </c>
-      <c r="P7" s="3" t="str">
+      <c r="P7" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "illuminance": {"measurement_type": 0x05, "accuracy_decimals": 2, "unit_of_measurement":"lux" , "device_class": DEVICE_CLASS_ILLUMINANCE},</v>
       </c>
@@ -1492,7 +1928,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "mass_kg": 0x06,</v>
       </c>
-      <c r="P8" s="3" t="str">
+      <c r="P8" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "mass_kg": {"measurement_type": 0x06, "accuracy_decimals": 2, "unit_of_measurement":"kg" , "device_class": DEVICE_CLASS_EMPTY},</v>
       </c>
@@ -1545,7 +1981,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "mass_lb": 0x07,</v>
       </c>
-      <c r="P9" s="3" t="str">
+      <c r="P9" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "mass_lb": {"measurement_type": 0x07, "accuracy_decimals": 2, "unit_of_measurement":"lb" , "device_class": DEVICE_CLASS_EMPTY},</v>
       </c>
@@ -1598,7 +2034,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "dewpoint": 0x08,</v>
       </c>
-      <c r="P10" s="3" t="str">
+      <c r="P10" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "dewpoint": {"measurement_type": 0x08, "accuracy_decimals": 2, "unit_of_measurement":"°C" , "device_class": DEVICE_CLASS_EMPTY},</v>
       </c>
@@ -1644,7 +2080,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "count": 0x09,</v>
       </c>
-      <c r="P11" s="3" t="str">
+      <c r="P11" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "count": {"measurement_type": 0x09, "accuracy_decimals": 0, "unit_of_measurement":"" , "device_class": DEVICE_CLASS_EMPTY},</v>
       </c>
@@ -1697,7 +2133,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "energy": 0x0A,</v>
       </c>
-      <c r="P12" s="3" t="str">
+      <c r="P12" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "energy": {"measurement_type": 0x0A, "accuracy_decimals": 3, "unit_of_measurement":"kWh" , "device_class": DEVICE_CLASS_ENERGY},</v>
       </c>
@@ -1750,7 +2186,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "power": 0x0B,</v>
       </c>
-      <c r="P13" s="3" t="str">
+      <c r="P13" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "power": {"measurement_type": 0x0B, "accuracy_decimals": 2, "unit_of_measurement":"W" , "device_class": DEVICE_CLASS_POWER},</v>
       </c>
@@ -1803,7 +2239,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "voltage": 0x0C,</v>
       </c>
-      <c r="P14" s="3" t="str">
+      <c r="P14" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "voltage": {"measurement_type": 0x0C, "accuracy_decimals": 3, "unit_of_measurement":"V" , "device_class": DEVICE_CLASS_VOLTAGE},</v>
       </c>
@@ -1852,7 +2288,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "pm2_5": 0x0D,</v>
       </c>
-      <c r="P15" s="3" t="str">
+      <c r="P15" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "pm2_5": {"measurement_type": 0x0D, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3" , "device_class": DEVICE_CLASS_PM25},</v>
       </c>
@@ -1901,7 +2337,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "pm10": 0x0E,</v>
       </c>
-      <c r="P16" s="3" t="str">
+      <c r="P16" t="str">
         <f t="shared" si="4"/>
         <v xml:space="preserve">    "pm10": {"measurement_type": 0x0E, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3" , "device_class": DEVICE_CLASS_PM10},</v>
       </c>
@@ -1945,7 +2381,7 @@
         <v xml:space="preserve">    "generic_boolean": 0x0F,</v>
       </c>
       <c r="P17" t="str">
-        <f t="shared" ref="P3:P49" si="6">"    """&amp;N17&amp;""": {""measurement_type"": " &amp; B17 &amp; ", ""accuracy_decimals"": "&amp;K17&amp;", ""unit_of_measurement"":"""&amp;H17&amp;"""},"</f>
+        <f t="shared" ref="P17:P47" si="6">"    """&amp;N17&amp;""": {""measurement_type"": " &amp; B17 &amp; ", ""accuracy_decimals"": "&amp;K17&amp;", ""unit_of_measurement"":"""&amp;H17&amp;"""},"</f>
         <v xml:space="preserve">    "generic_boolean": {"measurement_type": 0x0F, "accuracy_decimals": 0, "unit_of_measurement":""},</v>
       </c>
     </row>
@@ -2079,7 +2515,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "co2": 0x12,</v>
       </c>
-      <c r="P20" s="3" t="str">
+      <c r="P20" t="str">
         <f t="shared" ref="P20:P22" si="7">"    """&amp;N20&amp;""": {""measurement_type"": " &amp; B20 &amp; ", ""accuracy_decimals"": "&amp;K20&amp;", ""unit_of_measurement"":"""&amp;H20&amp;""" , ""device_class"": "&amp;I20&amp;"},"</f>
         <v xml:space="preserve">    "co2": {"measurement_type": 0x12, "accuracy_decimals": 0, "unit_of_measurement":"ppm" , "device_class": DEVICE_CLASS_CARBON_DIOXIDE},</v>
       </c>
@@ -2128,7 +2564,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "tvoc": 0x13,</v>
       </c>
-      <c r="P21" s="3" t="str">
+      <c r="P21" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">    "tvoc": {"measurement_type": 0x13, "accuracy_decimals": 0, "unit_of_measurement":"ug/m3" , "device_class": DEVICE_CLASS_VOLATILE_ORGANIC_COMPOUNDS},</v>
       </c>
@@ -2181,7 +2617,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "moisture": 0x14,</v>
       </c>
-      <c r="P22" s="3" t="str">
+      <c r="P22" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve">    "moisture": {"measurement_type": 0x14, "accuracy_decimals": 2, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_MOISTURE},</v>
       </c>
@@ -3305,7 +3741,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "humidity2": 0x2E,</v>
       </c>
-      <c r="P48" s="3" t="str">
+      <c r="P48" t="str">
         <f t="shared" ref="P48:P49" si="9">"    """&amp;N48&amp;""": {""measurement_type"": " &amp; B48 &amp; ", ""accuracy_decimals"": "&amp;K48&amp;", ""unit_of_measurement"":"""&amp;H48&amp;""" , ""device_class"": "&amp;I48&amp;"},"</f>
         <v xml:space="preserve">    "humidity2": {"measurement_type": 0x2E, "accuracy_decimals": 0, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_HUMIDITY},</v>
       </c>
@@ -3354,7 +3790,7 @@
         <f t="shared" si="3"/>
         <v xml:space="preserve">    "moisture2": 0x2F,</v>
       </c>
-      <c r="P49" s="3" t="str">
+      <c r="P49" t="str">
         <f t="shared" si="9"/>
         <v xml:space="preserve">    "moisture2": {"measurement_type": 0x2F, "accuracy_decimals": 0, "unit_of_measurement":"%" , "device_class": DEVICE_CLASS_MOISTURE},</v>
       </c>
@@ -3561,4 +3997,4015 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28042196-756D-49C6-ACCE-21EFE4A952B1}">
+  <dimension ref="A1:N94"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" customWidth="1"/>
+    <col min="6" max="6" width="13" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8" customWidth="1"/>
+    <col min="13" max="13" width="9" customWidth="1"/>
+    <col min="14" max="14" width="62" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="4" customFormat="1" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f t="shared" ref="A2:A78" si="0">HEX2DEC(SUBSTITUTE(B2,"0x",""))</f>
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="G2" s="6">
+        <v>9</v>
+      </c>
+      <c r="I2" s="6" t="str">
+        <f>IF(L2&gt;0," || obj_meas_type == "&amp;B2,"")</f>
+        <v/>
+      </c>
+      <c r="J2" s="6">
+        <f>_xlfn.NUMBERVALUE(IFERROR(MID(D2,FIND("(",D2)+1,1),0))</f>
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <f>IF(MID(D2,1,4)="sint",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>IFERROR(ABS(LOG10(E2)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="6" t="str">
+        <f>DEC2HEX(J2+_xlfn.BITLSHIFT(K2,3)+_xlfn.BITLSHIFT(L2,5),2)</f>
+        <v>01</v>
+      </c>
+      <c r="N2" s="6" t="str">
+        <f>"0x"&amp;M2&amp;","&amp;CHAR(9)&amp;" // "&amp;B2&amp;" | "&amp;C2&amp;" | "&amp;D2&amp;" | datatype: "&amp;K2&amp;" | factor_exp10: "&amp;E2&amp;" | example: "&amp;F2</f>
+        <v>0x01,	 // 0x00 | packet id | uint8 (1 byte) | datatype: 0 | factor_exp10: 1 | example: 9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G3">
+        <v>97</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="6" t="str">
+        <f>IF(L3&gt;0," || obj_meas_type == "&amp;B3,"")</f>
+        <v/>
+      </c>
+      <c r="J3" s="6">
+        <f t="shared" ref="J3:J66" si="1">_xlfn.NUMBERVALUE(IFERROR(MID(D3,FIND("(",D3)+1,1),0))</f>
+        <v>1</v>
+      </c>
+      <c r="K3" s="6">
+        <f t="shared" ref="K3:K66" si="2">IF(MID(D3,1,4)="sint",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f>IFERROR(ABS(LOG10(E3)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M3" s="6" t="str">
+        <f t="shared" ref="M3:M66" si="3">DEC2HEX(J3+_xlfn.BITLSHIFT(K3,3)+_xlfn.BITLSHIFT(L3,5),2)</f>
+        <v>01</v>
+      </c>
+      <c r="N3" s="6" t="str">
+        <f t="shared" ref="N3:N66" si="4">"0x"&amp;M3&amp;","&amp;CHAR(9)&amp;" // "&amp;B3&amp;" | "&amp;C3&amp;" | "&amp;D3&amp;" | datatype: "&amp;K3&amp;" | factor_exp10: "&amp;E3&amp;" | example: "&amp;F3</f>
+        <v>0x01,	 // 0x01 | battery | uint8 (1 byte) | datatype: 0 | factor_exp10: 1 | example: 0161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4">
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="G4">
+        <v>25.06</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="6" t="str">
+        <f>IF(L4&gt;0," || obj_meas_type == "&amp;B4,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x02</v>
+      </c>
+      <c r="J4" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K4" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f>IFERROR(ABS(LOG10(E4)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M4" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>4A</v>
+      </c>
+      <c r="N4" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x4A,	 // 0x02 | temperature | sint16 (2 bytes) | datatype: 1 | factor_exp10: 0.01 | example: 02CA09</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5">
+        <v>0.01</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="G5">
+        <v>50.55</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f>IF(L5&gt;0," || obj_meas_type == "&amp;B5,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x03</v>
+      </c>
+      <c r="J5" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K5" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <f>IFERROR(ABS(LOG10(E5)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M5" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="N5" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x42,	 // 0x03 | humidity | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.01 | example: 03BF13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E6">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="G6">
+        <v>1008.83</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="6" t="str">
+        <f>IF(L6&gt;0," || obj_meas_type == "&amp;B6,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x04</v>
+      </c>
+      <c r="J6" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K6" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <f>IFERROR(ABS(LOG10(E6)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M6" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="N6" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x43,	 // 0x04 | pressure | uint24 (3 bytes) | datatype: 0 | factor_exp10: 0.01 | example: 04138A01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E7">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="G7">
+        <v>13460.67</v>
+      </c>
+      <c r="H7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="6" t="str">
+        <f>IF(L7&gt;0," || obj_meas_type == "&amp;B7,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x05</v>
+      </c>
+      <c r="J7" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K7" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <f>IFERROR(ABS(LOG10(E7)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M7" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="N7" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x43,	 // 0x05 | illuminance | uint24 (3 bytes) | datatype: 0 | factor_exp10: 0.01 | example: 05138A14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>184</v>
+      </c>
+      <c r="E8">
+        <v>0.01</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="G8">
+        <v>80.3</v>
+      </c>
+      <c r="H8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I8" s="6" t="str">
+        <f>IF(L8&gt;0," || obj_meas_type == "&amp;B8,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x06</v>
+      </c>
+      <c r="J8" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K8" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>IFERROR(ABS(LOG10(E8)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M8" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="N8" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x42,	 // 0x06 | mass (kg) | uint16 (2 byte) | datatype: 0 | factor_exp10: 0.01 | example: 065E1F</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E9">
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="G9">
+        <v>74.86</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="6" t="str">
+        <f>IF(L9&gt;0," || obj_meas_type == "&amp;B9,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x07</v>
+      </c>
+      <c r="J9" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <f>IFERROR(ABS(LOG10(E9)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M9" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="N9" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x42,	 // 0x07 | mass (lb) | uint16 (2 byte) | datatype: 0 | factor_exp10: 0.01 | example: 073E1D</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10">
+        <v>0.01</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10">
+        <v>17.38</v>
+      </c>
+      <c r="H10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="6" t="str">
+        <f>IF(L10&gt;0," || obj_meas_type == "&amp;B10,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x08</v>
+      </c>
+      <c r="J10" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L10">
+        <f>IFERROR(ABS(LOG10(E10)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M10" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>4A</v>
+      </c>
+      <c r="N10" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x4A,	 // 0x08 | dewpoint | sint16 (2 bytes) | datatype: 1 | factor_exp10: 0.01 | example: 08CA06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" t="s">
+        <v>219</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="G11">
+        <v>96</v>
+      </c>
+      <c r="I11" s="6" t="str">
+        <f>IF(L11&gt;0," || obj_meas_type == "&amp;B11,"")</f>
+        <v/>
+      </c>
+      <c r="J11" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>IFERROR(ABS(LOG10(E11)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N11" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x09 | count | uint (1 bytes) | datatype: 0 | factor_exp10: 1 | example: 0960</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>183</v>
+      </c>
+      <c r="E12">
+        <v>1E-3</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="G12">
+        <v>1346.067</v>
+      </c>
+      <c r="H12" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="6" t="str">
+        <f>IF(L12&gt;0," || obj_meas_type == "&amp;B12,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x0A</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f>IFERROR(ABS(LOG10(E12)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M12" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="N12" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x63,	 // 0x0A | energy | uint24 (3 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 0A138A14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13">
+        <v>0.01</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="G13">
+        <v>69.14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I13" s="6" t="str">
+        <f>IF(L13&gt;0," || obj_meas_type == "&amp;B13,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x0B</v>
+      </c>
+      <c r="J13" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="K13" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>IFERROR(ABS(LOG10(E13)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M13" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="N13" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x43,	 // 0x0B | power | uint24 (3 bytes) | datatype: 0 | factor_exp10: 0.01 | example: 0B021B00</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>182</v>
+      </c>
+      <c r="E14">
+        <v>1E-3</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="G14">
+        <v>3.0739999999999998</v>
+      </c>
+      <c r="H14" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="6" t="str">
+        <f>IF(L14&gt;0," || obj_meas_type == "&amp;B14,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x0C</v>
+      </c>
+      <c r="J14" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K14" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>IFERROR(ABS(LOG10(E14)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M14" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="N14" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x62,	 // 0x0C | voltage | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 0C020C</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="G15">
+        <v>3090</v>
+      </c>
+      <c r="H15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="6" t="str">
+        <f>IF(L15&gt;0," || obj_meas_type == "&amp;B15,"")</f>
+        <v/>
+      </c>
+      <c r="J15" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K15" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>IFERROR(ABS(LOG10(E15)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M15" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>02</v>
+      </c>
+      <c r="N15" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x02,	 // 0x0D | pm2.5 | uint16 (2 bytes) | datatype: 0 | factor_exp10: 1 | example: 0D120C</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" t="s">
+        <v>182</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="G16">
+        <v>7170</v>
+      </c>
+      <c r="H16" t="s">
+        <v>52</v>
+      </c>
+      <c r="I16" s="6" t="str">
+        <f>IF(L16&gt;0," || obj_meas_type == "&amp;B16,"")</f>
+        <v/>
+      </c>
+      <c r="J16" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K16" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>IFERROR(ABS(LOG10(E16)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>02</v>
+      </c>
+      <c r="N16" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x02,	 // 0x0E | pm10 | uint16 (2 bytes) | datatype: 0 | factor_exp10: 1 | example: 0E021C</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>302</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I17" s="6" t="str">
+        <f>IF(L17&gt;0," || obj_meas_type == "&amp;B17,"")</f>
+        <v/>
+      </c>
+      <c r="J17" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K17" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>IFERROR(ABS(LOG10(E17)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M17" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N17" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x0F | generic boolean | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 0F01</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18">
+        <v>1001</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I18" s="6" t="str">
+        <f>IF(L18&gt;0," || obj_meas_type == "&amp;B18,"")</f>
+        <v/>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>IFERROR(ABS(LOG10(E18)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M18" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N18" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x10 | power | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19">
+        <v>1100</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I19" s="6" t="str">
+        <f>IF(L19&gt;0," || obj_meas_type == "&amp;B19,"")</f>
+        <v/>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>IFERROR(ABS(LOG10(E19)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N19" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x11 | opening | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" t="s">
+        <v>182</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="G20">
+        <v>1250</v>
+      </c>
+      <c r="H20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I20" s="6" t="str">
+        <f>IF(L20&gt;0," || obj_meas_type == "&amp;B20,"")</f>
+        <v/>
+      </c>
+      <c r="J20" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K20" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>IFERROR(ABS(LOG10(E20)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M20" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>02</v>
+      </c>
+      <c r="N20" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x02,	 // 0x12 | co2 | uint16 (2 bytes) | datatype: 0 | factor_exp10: 1 | example: 12E204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>182</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="G21">
+        <v>307</v>
+      </c>
+      <c r="H21" t="s">
+        <v>52</v>
+      </c>
+      <c r="I21" s="6" t="str">
+        <f>IF(L21&gt;0," || obj_meas_type == "&amp;B21,"")</f>
+        <v/>
+      </c>
+      <c r="J21" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K21" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>IFERROR(ABS(LOG10(E21)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>02</v>
+      </c>
+      <c r="N21" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x02,	 // 0x13 | tvoc | uint16 (2 bytes) | datatype: 0 | factor_exp10: 1 | example: 133301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>182</v>
+      </c>
+      <c r="E22">
+        <v>0.01</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="G22">
+        <v>30.74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" s="6" t="str">
+        <f>IF(L22&gt;0," || obj_meas_type == "&amp;B22,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x14</v>
+      </c>
+      <c r="J22" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K22" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>IFERROR(ABS(LOG10(E22)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M22" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="N22" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x42,	 // 0x14 | moisture | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.01 | example: 14020C</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23">
+        <v>1501</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="I23" s="6" t="str">
+        <f>IF(L23&gt;0," || obj_meas_type == "&amp;B23,"")</f>
+        <v/>
+      </c>
+      <c r="J23" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K23" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>IFERROR(ABS(LOG10(E23)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N23" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x15 | battery | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1501</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24">
+        <v>1601</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="I24" s="6" t="str">
+        <f>IF(L24&gt;0," || obj_meas_type == "&amp;B24,"")</f>
+        <v/>
+      </c>
+      <c r="J24" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K24" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>IFERROR(ABS(LOG10(E24)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N24" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x16 | battery charging | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1601</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>80</v>
+      </c>
+      <c r="C25" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F25">
+        <v>1700</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I25" s="6" t="str">
+        <f>IF(L25&gt;0," || obj_meas_type == "&amp;B25,"")</f>
+        <v/>
+      </c>
+      <c r="J25" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K25" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>IFERROR(ABS(LOG10(E25)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M25" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N25" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x17 | carbon monoxide | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1700</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26">
+        <v>1801</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="I26" s="6" t="str">
+        <f>IF(L26&gt;0," || obj_meas_type == "&amp;B26,"")</f>
+        <v/>
+      </c>
+      <c r="J26" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K26" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>IFERROR(ABS(LOG10(E26)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M26" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N26" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x18 | cold | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1801</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27">
+        <v>1900</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="I27" s="6" t="str">
+        <f>IF(L27&gt;0," || obj_meas_type == "&amp;B27,"")</f>
+        <v/>
+      </c>
+      <c r="J27" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K27" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>IFERROR(ABS(LOG10(E27)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M27" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N27" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x19 | connectivity | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1900</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
+        <v>90</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="F28" t="s">
+        <v>299</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I28" s="6" t="str">
+        <f>IF(L28&gt;0," || obj_meas_type == "&amp;B28,"")</f>
+        <v/>
+      </c>
+      <c r="J28" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K28" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>IFERROR(ABS(LOG10(E28)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M28" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N28" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x1A | door | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1A00</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" t="s">
+        <v>300</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I29" s="6" t="str">
+        <f>IF(L29&gt;0," || obj_meas_type == "&amp;B29,"")</f>
+        <v/>
+      </c>
+      <c r="J29" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K29" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <f>IFERROR(ABS(LOG10(E29)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N29" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x1B | garage door | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1B01</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" t="s">
+        <v>68</v>
+      </c>
+      <c r="F30" t="s">
+        <v>301</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I30" s="6" t="str">
+        <f>IF(L30&gt;0," || obj_meas_type == "&amp;B30,"")</f>
+        <v/>
+      </c>
+      <c r="J30" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K30" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L30">
+        <f>IFERROR(ABS(LOG10(E30)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M30" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N30" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x1C | gas | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1C01</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>99</v>
+      </c>
+      <c r="C31" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" t="s">
+        <v>303</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="I31" s="6" t="str">
+        <f>IF(L31&gt;0," || obj_meas_type == "&amp;B31,"")</f>
+        <v/>
+      </c>
+      <c r="J31" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L31">
+        <f>IFERROR(ABS(LOG10(E31)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N31" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x1D | heat | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1D00</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+      <c r="C32" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" t="s">
+        <v>68</v>
+      </c>
+      <c r="F32" s="1">
+        <v>10</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="I32" s="6" t="str">
+        <f>IF(L32&gt;0," || obj_meas_type == "&amp;B32,"")</f>
+        <v/>
+      </c>
+      <c r="J32" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K32" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <f>IFERROR(ABS(LOG10(E32)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N32" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x1E | light | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
+        <v>68</v>
+      </c>
+      <c r="F33" t="s">
+        <v>304</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="I33" s="6" t="str">
+        <f>IF(L33&gt;0," || obj_meas_type == "&amp;B33,"")</f>
+        <v/>
+      </c>
+      <c r="J33" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K33" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <f>IFERROR(ABS(LOG10(E33)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N33" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x1F | lock | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 1F01</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F34">
+        <v>2001</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="I34" s="6" t="str">
+        <f>IF(L34&gt;0," || obj_meas_type == "&amp;B34,"")</f>
+        <v/>
+      </c>
+      <c r="J34" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K34" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L34">
+        <f>IFERROR(ABS(LOG10(E34)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M34" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N34" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x20 | moisture | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>112</v>
+      </c>
+      <c r="C35" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" t="s">
+        <v>68</v>
+      </c>
+      <c r="F35">
+        <v>2100</v>
+      </c>
+      <c r="G35" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I35" s="6" t="str">
+        <f>IF(L35&gt;0," || obj_meas_type == "&amp;B35,"")</f>
+        <v/>
+      </c>
+      <c r="J35" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <f>IFERROR(ABS(LOG10(E35)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M35" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N35" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x21 | motion | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" t="s">
+        <v>68</v>
+      </c>
+      <c r="F36">
+        <v>2201</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="I36" s="6" t="str">
+        <f>IF(L36&gt;0," || obj_meas_type == "&amp;B36,"")</f>
+        <v/>
+      </c>
+      <c r="J36" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <f>IFERROR(ABS(LOG10(E36)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M36" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N36" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x22 | moving | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" t="s">
+        <v>68</v>
+      </c>
+      <c r="F37">
+        <v>2301</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I37" s="6" t="str">
+        <f>IF(L37&gt;0," || obj_meas_type == "&amp;B37,"")</f>
+        <v/>
+      </c>
+      <c r="J37" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <f>IFERROR(ABS(LOG10(E37)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M37" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N37" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x23 | occupancy | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2301</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" t="s">
+        <v>121</v>
+      </c>
+      <c r="D38" t="s">
+        <v>68</v>
+      </c>
+      <c r="F38">
+        <v>2400</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="I38" s="6" t="str">
+        <f>IF(L38&gt;0," || obj_meas_type == "&amp;B38,"")</f>
+        <v/>
+      </c>
+      <c r="J38" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K38" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L38">
+        <f>IFERROR(ABS(LOG10(E38)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M38" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N38" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x24 | plug | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2400</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F39">
+        <v>2500</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="I39" s="6" t="str">
+        <f>IF(L39&gt;0," || obj_meas_type == "&amp;B39,"")</f>
+        <v/>
+      </c>
+      <c r="J39" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K39" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L39">
+        <f>IFERROR(ABS(LOG10(E39)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N39" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x25 | presence | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2500</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B40" t="s">
+        <v>126</v>
+      </c>
+      <c r="C40" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" t="s">
+        <v>68</v>
+      </c>
+      <c r="F40">
+        <v>2601</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="I40" s="6" t="str">
+        <f>IF(L40&gt;0," || obj_meas_type == "&amp;B40,"")</f>
+        <v/>
+      </c>
+      <c r="J40" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K40" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <f>IFERROR(ABS(LOG10(E40)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M40" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N40" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x26 | problem | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2601</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>129</v>
+      </c>
+      <c r="C41" t="s">
+        <v>130</v>
+      </c>
+      <c r="D41" t="s">
+        <v>68</v>
+      </c>
+      <c r="F41">
+        <v>2701</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="I41" s="6" t="str">
+        <f>IF(L41&gt;0," || obj_meas_type == "&amp;B41,"")</f>
+        <v/>
+      </c>
+      <c r="J41" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K41" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L41">
+        <f>IFERROR(ABS(LOG10(E41)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M41" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N41" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x27 | running | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2701</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>132</v>
+      </c>
+      <c r="C42" t="s">
+        <v>133</v>
+      </c>
+      <c r="D42" t="s">
+        <v>68</v>
+      </c>
+      <c r="F42">
+        <v>2800</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="I42" s="6" t="str">
+        <f>IF(L42&gt;0," || obj_meas_type == "&amp;B42,"")</f>
+        <v/>
+      </c>
+      <c r="J42" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K42" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <f>IFERROR(ABS(LOG10(E42)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M42" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N42" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x28 | safety | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2800</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>135</v>
+      </c>
+      <c r="C43" t="s">
+        <v>136</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+      <c r="F43">
+        <v>2901</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I43" s="6" t="str">
+        <f>IF(L43&gt;0," || obj_meas_type == "&amp;B43,"")</f>
+        <v/>
+      </c>
+      <c r="J43" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K43" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L43">
+        <f>IFERROR(ABS(LOG10(E43)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M43" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N43" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x29 | smoke | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2901</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>137</v>
+      </c>
+      <c r="C44" t="s">
+        <v>138</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" t="s">
+        <v>305</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I44" s="6" t="str">
+        <f>IF(L44&gt;0," || obj_meas_type == "&amp;B44,"")</f>
+        <v/>
+      </c>
+      <c r="J44" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K44" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <f>IFERROR(ABS(LOG10(E44)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M44" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N44" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x2A | sound | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2A00</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>140</v>
+      </c>
+      <c r="C45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D45" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" t="s">
+        <v>306</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="I45" s="6" t="str">
+        <f>IF(L45&gt;0," || obj_meas_type == "&amp;B45,"")</f>
+        <v/>
+      </c>
+      <c r="J45" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K45" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <f>IFERROR(ABS(LOG10(E45)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M45" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N45" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x2B | tamper | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2B00</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" t="s">
+        <v>145</v>
+      </c>
+      <c r="D46" t="s">
+        <v>68</v>
+      </c>
+      <c r="F46" t="s">
+        <v>307</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I46" s="6" t="str">
+        <f>IF(L46&gt;0," || obj_meas_type == "&amp;B46,"")</f>
+        <v/>
+      </c>
+      <c r="J46" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K46" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <f>IFERROR(ABS(LOG10(E46)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M46" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N46" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x2C | vibration | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2C01</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>147</v>
+      </c>
+      <c r="C47" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" t="s">
+        <v>68</v>
+      </c>
+      <c r="F47" t="s">
+        <v>308</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="I47" s="6" t="str">
+        <f>IF(L47&gt;0," || obj_meas_type == "&amp;B47,"")</f>
+        <v/>
+      </c>
+      <c r="J47" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K47" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <f>IFERROR(ABS(LOG10(E47)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M47" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N47" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x2D | window | uint8 (1 byte) | datatype: 0 | factor_exp10:  | example: 2D01</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>16</v>
+      </c>
+      <c r="C48" t="s">
+        <v>14</v>
+      </c>
+      <c r="D48" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="G48">
+        <v>35</v>
+      </c>
+      <c r="H48" t="s">
+        <v>8</v>
+      </c>
+      <c r="I48" s="6" t="str">
+        <f>IF(L48&gt;0," || obj_meas_type == "&amp;B48,"")</f>
+        <v/>
+      </c>
+      <c r="J48" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K48" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <f>IFERROR(ABS(LOG10(E48)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M48" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N48" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x2E | humidity | uint8 (1 byte) | datatype: 0 | factor_exp10: 1 | example: 2E23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G49">
+        <v>35</v>
+      </c>
+      <c r="H49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I49" s="6" t="str">
+        <f>IF(L49&gt;0," || obj_meas_type == "&amp;B49,"")</f>
+        <v/>
+      </c>
+      <c r="J49" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K49" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <f>IFERROR(ABS(LOG10(E49)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M49" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="N49" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x01,	 // 0x2F | moisture | uint8 (1 byte) | datatype: 0 | factor_exp10: 1 | example: 2F23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>339</v>
+      </c>
+      <c r="C50" t="s">
+        <v>350</v>
+      </c>
+      <c r="I50" s="6" t="str">
+        <f>IF(L50&gt;0," || obj_meas_type == "&amp;B50,"")</f>
+        <v/>
+      </c>
+      <c r="J50" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K50" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <f>IFERROR(ABS(LOG10(E50)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M50" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N50" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x30 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>340</v>
+      </c>
+      <c r="C51" t="s">
+        <v>350</v>
+      </c>
+      <c r="I51" s="6" t="str">
+        <f>IF(L51&gt;0," || obj_meas_type == "&amp;B51,"")</f>
+        <v/>
+      </c>
+      <c r="J51" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K51" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <f>IFERROR(ABS(LOG10(E51)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M51" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N51" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x31 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>341</v>
+      </c>
+      <c r="C52" t="s">
+        <v>350</v>
+      </c>
+      <c r="I52" s="6" t="str">
+        <f>IF(L52&gt;0," || obj_meas_type == "&amp;B52,"")</f>
+        <v/>
+      </c>
+      <c r="J52" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K52" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <f>IFERROR(ABS(LOG10(E52)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M52" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N52" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x32 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>342</v>
+      </c>
+      <c r="C53" t="s">
+        <v>350</v>
+      </c>
+      <c r="I53" s="6" t="str">
+        <f>IF(L53&gt;0," || obj_meas_type == "&amp;B53,"")</f>
+        <v/>
+      </c>
+      <c r="J53" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K53" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <f>IFERROR(ABS(LOG10(E53)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M53" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N53" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x33 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>343</v>
+      </c>
+      <c r="C54" t="s">
+        <v>350</v>
+      </c>
+      <c r="I54" s="6" t="str">
+        <f>IF(L54&gt;0," || obj_meas_type == "&amp;B54,"")</f>
+        <v/>
+      </c>
+      <c r="J54" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <f>IFERROR(ABS(LOG10(E54)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M54" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N54" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x34 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>344</v>
+      </c>
+      <c r="C55" t="s">
+        <v>350</v>
+      </c>
+      <c r="I55" s="6" t="str">
+        <f>IF(L55&gt;0," || obj_meas_type == "&amp;B55,"")</f>
+        <v/>
+      </c>
+      <c r="J55" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K55" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <f>IFERROR(ABS(LOG10(E55)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M55" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N55" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x35 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>345</v>
+      </c>
+      <c r="C56" t="s">
+        <v>350</v>
+      </c>
+      <c r="I56" s="6" t="str">
+        <f>IF(L56&gt;0," || obj_meas_type == "&amp;B56,"")</f>
+        <v/>
+      </c>
+      <c r="J56" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <f>IFERROR(ABS(LOG10(E56)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M56" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N56" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x36 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>346</v>
+      </c>
+      <c r="C57" t="s">
+        <v>350</v>
+      </c>
+      <c r="I57" s="6" t="str">
+        <f>IF(L57&gt;0," || obj_meas_type == "&amp;B57,"")</f>
+        <v/>
+      </c>
+      <c r="J57" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K57" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L57">
+        <f>IFERROR(ABS(LOG10(E57)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M57" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N57" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x37 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>347</v>
+      </c>
+      <c r="C58" t="s">
+        <v>350</v>
+      </c>
+      <c r="I58" s="6" t="str">
+        <f>IF(L58&gt;0," || obj_meas_type == "&amp;B58,"")</f>
+        <v/>
+      </c>
+      <c r="J58" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K58" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <f>IFERROR(ABS(LOG10(E58)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M58" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N58" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x38 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>348</v>
+      </c>
+      <c r="C59" t="s">
+        <v>350</v>
+      </c>
+      <c r="I59" s="6" t="str">
+        <f>IF(L59&gt;0," || obj_meas_type == "&amp;B59,"")</f>
+        <v/>
+      </c>
+      <c r="J59" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K59" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <f>IFERROR(ABS(LOG10(E59)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M59" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N59" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x39 | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>152</v>
+      </c>
+      <c r="C60" t="s">
+        <v>351</v>
+      </c>
+      <c r="F60"/>
+      <c r="I60" s="6" t="str">
+        <f>IF(L60&gt;0," || obj_meas_type == "&amp;B60,"")</f>
+        <v/>
+      </c>
+      <c r="J60" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K60" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L60">
+        <f>IFERROR(ABS(LOG10(E60)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M60" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N60" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x3A | TODO |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>349</v>
+      </c>
+      <c r="C61" t="s">
+        <v>350</v>
+      </c>
+      <c r="I61" s="6" t="str">
+        <f>IF(L61&gt;0," || obj_meas_type == "&amp;B61,"")</f>
+        <v/>
+      </c>
+      <c r="J61" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K61" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L61">
+        <f>IFERROR(ABS(LOG10(E61)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M61" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N61" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x3B | NA |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>168</v>
+      </c>
+      <c r="C62" t="s">
+        <v>351</v>
+      </c>
+      <c r="I62" s="6" t="str">
+        <f>IF(L62&gt;0," || obj_meas_type == "&amp;B62,"")</f>
+        <v/>
+      </c>
+      <c r="J62" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K62" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L62">
+        <f>IFERROR(ABS(LOG10(E62)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M62" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>00</v>
+      </c>
+      <c r="N62" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve">0x00,	 // 0x3C | TODO |  | datatype: 0 | factor_exp10:  | example: </v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>220</v>
+      </c>
+      <c r="C63" t="s">
+        <v>37</v>
+      </c>
+      <c r="D63" t="s">
+        <v>221</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G63">
+        <v>24585</v>
+      </c>
+      <c r="I63" s="6" t="str">
+        <f>IF(L63&gt;0," || obj_meas_type == "&amp;B63,"")</f>
+        <v/>
+      </c>
+      <c r="J63" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K63" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <f>IFERROR(ABS(LOG10(E63)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M63" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>02</v>
+      </c>
+      <c r="N63" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x02,	 // 0x3D | count | uint (2 bytes) | datatype: 0 | factor_exp10: 1 | example: 3D0960</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>223</v>
+      </c>
+      <c r="C64" t="s">
+        <v>37</v>
+      </c>
+      <c r="D64" t="s">
+        <v>185</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="G64">
+        <v>1611213866</v>
+      </c>
+      <c r="I64" s="6" t="str">
+        <f>IF(L64&gt;0," || obj_meas_type == "&amp;B64,"")</f>
+        <v/>
+      </c>
+      <c r="J64" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K64" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <f>IFERROR(ABS(LOG10(E64)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M64" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>04</v>
+      </c>
+      <c r="N64" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x04,	 // 0x3E | count | uint (4 bytes) | datatype: 0 | factor_exp10: 1 | example: 3E2A2C0960</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>259</v>
+      </c>
+      <c r="C65" t="s">
+        <v>260</v>
+      </c>
+      <c r="D65" t="s">
+        <v>181</v>
+      </c>
+      <c r="E65">
+        <v>0.1</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G65">
+        <v>307.39999999999998</v>
+      </c>
+      <c r="H65" t="s">
+        <v>262</v>
+      </c>
+      <c r="I65" s="6" t="str">
+        <f>IF(L65&gt;0," || obj_meas_type == "&amp;B65,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x3F</v>
+      </c>
+      <c r="J65" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K65" s="6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="L65">
+        <f>IFERROR(ABS(LOG10(E65)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M65" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>2A</v>
+      </c>
+      <c r="N65" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x2A,	 // 0x3F | rotation | sint16 (2 bytes) | datatype: 1 | factor_exp10: 0.1 | example: 3F020C</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>229</v>
+      </c>
+      <c r="C66" t="s">
+        <v>230</v>
+      </c>
+      <c r="D66" t="s">
+        <v>182</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="G66">
+        <v>12</v>
+      </c>
+      <c r="H66" t="s">
+        <v>232</v>
+      </c>
+      <c r="I66" s="6" t="str">
+        <f>IF(L66&gt;0," || obj_meas_type == "&amp;B66,"")</f>
+        <v/>
+      </c>
+      <c r="J66" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="K66" s="6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <f>IFERROR(ABS(LOG10(E66)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M66" s="6" t="str">
+        <f t="shared" si="3"/>
+        <v>02</v>
+      </c>
+      <c r="N66" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>0x02,	 // 0x40 | distance (mm) | uint16 (2 bytes) | datatype: 0 | factor_exp10: 1 | example: 400C00</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>233</v>
+      </c>
+      <c r="C67" t="s">
+        <v>234</v>
+      </c>
+      <c r="D67" t="s">
+        <v>182</v>
+      </c>
+      <c r="E67">
+        <v>0.1</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G67">
+        <v>7.8</v>
+      </c>
+      <c r="H67" t="s">
+        <v>235</v>
+      </c>
+      <c r="I67" s="6" t="str">
+        <f>IF(L67&gt;0," || obj_meas_type == "&amp;B67,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x41</v>
+      </c>
+      <c r="J67" s="6">
+        <f t="shared" ref="J67:J81" si="5">_xlfn.NUMBERVALUE(IFERROR(MID(D67,FIND("(",D67)+1,1),0))</f>
+        <v>2</v>
+      </c>
+      <c r="K67" s="6">
+        <f t="shared" ref="K67:K81" si="6">IF(MID(D67,1,4)="sint",1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <f>IFERROR(ABS(LOG10(E67)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M67" s="6" t="str">
+        <f t="shared" ref="M67:M81" si="7">DEC2HEX(J67+_xlfn.BITLSHIFT(K67,3)+_xlfn.BITLSHIFT(L67,5),2)</f>
+        <v>22</v>
+      </c>
+      <c r="N67" s="6" t="str">
+        <f t="shared" ref="N67:N81" si="8">"0x"&amp;M67&amp;","&amp;CHAR(9)&amp;" // "&amp;B67&amp;" | "&amp;C67&amp;" | "&amp;D67&amp;" | datatype: "&amp;K67&amp;" | factor_exp10: "&amp;E67&amp;" | example: "&amp;F67</f>
+        <v>0x22,	 // 0x41 | distance (m) | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.1 | example: 414E00</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>236</v>
+      </c>
+      <c r="C68" t="s">
+        <v>237</v>
+      </c>
+      <c r="D68" t="s">
+        <v>183</v>
+      </c>
+      <c r="E68">
+        <v>1E-3</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="G68">
+        <v>13.39</v>
+      </c>
+      <c r="H68" t="s">
+        <v>239</v>
+      </c>
+      <c r="I68" s="6" t="str">
+        <f>IF(L68&gt;0," || obj_meas_type == "&amp;B68,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x42</v>
+      </c>
+      <c r="J68" s="6">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="K68" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <f>IFERROR(ABS(LOG10(E68)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M68" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>63</v>
+      </c>
+      <c r="N68" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x63,	 // 0x42 | duration | uint24 (3 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 424E3400</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>225</v>
+      </c>
+      <c r="C69" t="s">
+        <v>226</v>
+      </c>
+      <c r="D69" t="s">
+        <v>182</v>
+      </c>
+      <c r="E69">
+        <v>1E-3</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="G69">
+        <v>13.39</v>
+      </c>
+      <c r="H69" t="s">
+        <v>227</v>
+      </c>
+      <c r="I69" s="6" t="str">
+        <f>IF(L69&gt;0," || obj_meas_type == "&amp;B69,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x43</v>
+      </c>
+      <c r="J69" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K69" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L69">
+        <f>IFERROR(ABS(LOG10(E69)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M69" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>62</v>
+      </c>
+      <c r="N69" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x62,	 // 0x43 | current | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 434E34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>263</v>
+      </c>
+      <c r="C70" t="s">
+        <v>264</v>
+      </c>
+      <c r="D70" t="s">
+        <v>182</v>
+      </c>
+      <c r="E70">
+        <v>0.01</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="G70">
+        <v>133.9</v>
+      </c>
+      <c r="H70" t="s">
+        <v>265</v>
+      </c>
+      <c r="I70" s="6" t="str">
+        <f>IF(L70&gt;0," || obj_meas_type == "&amp;B70,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x44</v>
+      </c>
+      <c r="J70" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K70" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <f>IFERROR(ABS(LOG10(E70)),0)</f>
+        <v>2</v>
+      </c>
+      <c r="M70" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>42</v>
+      </c>
+      <c r="N70" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x42,	 // 0x44 | speed | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.01 | example: 444E34</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>266</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
+        <v>181</v>
+      </c>
+      <c r="E71">
+        <v>0.1</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="G71">
+        <v>27.3</v>
+      </c>
+      <c r="H71" t="s">
+        <v>12</v>
+      </c>
+      <c r="I71" s="6" t="str">
+        <f>IF(L71&gt;0," || obj_meas_type == "&amp;B71,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x45</v>
+      </c>
+      <c r="J71" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K71" s="6">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="L71">
+        <f>IFERROR(ABS(LOG10(E71)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M71" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>2A</v>
+      </c>
+      <c r="N71" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x2A,	 // 0x45 | temperature | sint16 (2 bytes) | datatype: 1 | factor_exp10: 0.1 | example: 451101</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>283</v>
+      </c>
+      <c r="C72" t="s">
+        <v>284</v>
+      </c>
+      <c r="D72" t="s">
+        <v>68</v>
+      </c>
+      <c r="E72">
+        <v>0.1</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G72">
+        <v>5</v>
+      </c>
+      <c r="I72" s="6" t="str">
+        <f>IF(L72&gt;0," || obj_meas_type == "&amp;B72,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x46</v>
+      </c>
+      <c r="J72" s="6">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="K72" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <f>IFERROR(ABS(LOG10(E72)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M72" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>21</v>
+      </c>
+      <c r="N72" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x21,	 // 0x46 | UV index | uint8 (1 byte) | datatype: 0 | factor_exp10: 0.1 | example: 4632</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="0"/>
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>275</v>
+      </c>
+      <c r="C73" t="s">
+        <v>272</v>
+      </c>
+      <c r="D73" t="s">
+        <v>182</v>
+      </c>
+      <c r="E73">
+        <v>0.1</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G73">
+        <v>2215.1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>274</v>
+      </c>
+      <c r="I73" s="6" t="str">
+        <f>IF(L73&gt;0," || obj_meas_type == "&amp;B73,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x47</v>
+      </c>
+      <c r="J73" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K73" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <f>IFERROR(ABS(LOG10(E73)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M73" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+      <c r="N73" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x22,	 // 0x47 | volume | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.1 | example: 478756</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>276</v>
+      </c>
+      <c r="C74" t="s">
+        <v>272</v>
+      </c>
+      <c r="D74" t="s">
+        <v>182</v>
+      </c>
+      <c r="E74">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="G74">
+        <v>34780</v>
+      </c>
+      <c r="H74" t="s">
+        <v>278</v>
+      </c>
+      <c r="I74" s="6" t="str">
+        <f>IF(L74&gt;0," || obj_meas_type == "&amp;B74,"")</f>
+        <v/>
+      </c>
+      <c r="J74" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K74" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <f>IFERROR(ABS(LOG10(E74)),0)</f>
+        <v>0</v>
+      </c>
+      <c r="M74" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>02</v>
+      </c>
+      <c r="N74" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x02,	 // 0x48 | volume | uint16 (2 bytes) | datatype: 0 | factor_exp10: 1 | example: 48DC87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="0"/>
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>279</v>
+      </c>
+      <c r="C75" t="s">
+        <v>280</v>
+      </c>
+      <c r="D75" t="s">
+        <v>182</v>
+      </c>
+      <c r="E75">
+        <v>1E-3</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G75">
+        <v>34.78</v>
+      </c>
+      <c r="H75" t="s">
+        <v>282</v>
+      </c>
+      <c r="I75" s="6" t="str">
+        <f>IF(L75&gt;0," || obj_meas_type == "&amp;B75,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x49</v>
+      </c>
+      <c r="J75" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K75" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <f>IFERROR(ABS(LOG10(E75)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M75" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>62</v>
+      </c>
+      <c r="N75" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x62,	 // 0x49 | volume Flow Rate | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 49DC87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>269</v>
+      </c>
+      <c r="C76" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" t="s">
+        <v>182</v>
+      </c>
+      <c r="E76">
+        <v>0.1</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="G76">
+        <v>307.39999999999998</v>
+      </c>
+      <c r="H76" t="s">
+        <v>48</v>
+      </c>
+      <c r="I76" s="6" t="str">
+        <f>IF(L76&gt;0," || obj_meas_type == "&amp;B76,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x4A</v>
+      </c>
+      <c r="J76" s="6">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="K76" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <f>IFERROR(ABS(LOG10(E76)),0)</f>
+        <v>1</v>
+      </c>
+      <c r="M76" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>22</v>
+      </c>
+      <c r="N76" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x22,	 // 0x4A | voltage | uint16 (2 bytes) | datatype: 0 | factor_exp10: 0.1 | example: 4A020C</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>244</v>
+      </c>
+      <c r="C77" t="s">
+        <v>96</v>
+      </c>
+      <c r="D77" t="s">
+        <v>183</v>
+      </c>
+      <c r="E77">
+        <v>1E-3</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="G77">
+        <v>1346.067</v>
+      </c>
+      <c r="H77" t="s">
+        <v>246</v>
+      </c>
+      <c r="I77" s="6" t="str">
+        <f>IF(L77&gt;0," || obj_meas_type == "&amp;B77,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x4B</v>
+      </c>
+      <c r="J77" s="6">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="K77" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L77">
+        <f>IFERROR(ABS(LOG10(E77)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M77" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>63</v>
+      </c>
+      <c r="N77" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x63,	 // 0x4B | gas | uint24 (3 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 4B138A14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="0"/>
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>247</v>
+      </c>
+      <c r="C78" t="s">
+        <v>96</v>
+      </c>
+      <c r="D78" t="s">
+        <v>241</v>
+      </c>
+      <c r="E78">
+        <v>1E-3</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="G78">
+        <v>25821.505000000001</v>
+      </c>
+      <c r="H78" t="s">
+        <v>246</v>
+      </c>
+      <c r="I78" s="6" t="str">
+        <f>IF(L78&gt;0," || obj_meas_type == "&amp;B78,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x4C</v>
+      </c>
+      <c r="J78" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K78" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <f>IFERROR(ABS(LOG10(E78)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M78" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="N78" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x64,	 // 0x4C | gas | uint32 (4 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 4C41018A01</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" ref="A79:A81" si="9">HEX2DEC(SUBSTITUTE(B79,"0x",""))</f>
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>240</v>
+      </c>
+      <c r="C79" t="s">
+        <v>38</v>
+      </c>
+      <c r="D79" t="s">
+        <v>241</v>
+      </c>
+      <c r="E79">
+        <v>1E-3</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="G79">
+        <v>344593.17</v>
+      </c>
+      <c r="H79" t="s">
+        <v>40</v>
+      </c>
+      <c r="I79" s="6" t="str">
+        <f>IF(L79&gt;0," || obj_meas_type == "&amp;B79,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x4D</v>
+      </c>
+      <c r="J79" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K79" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <f>IFERROR(ABS(LOG10(E79)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M79" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="N79" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x64,	 // 0x4D | energy | uint32 (4 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 4d12138a14</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="9"/>
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>271</v>
+      </c>
+      <c r="C80" t="s">
+        <v>272</v>
+      </c>
+      <c r="D80" t="s">
+        <v>241</v>
+      </c>
+      <c r="E80">
+        <v>1E-3</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="G80">
+        <v>19551.879000000001</v>
+      </c>
+      <c r="H80" t="s">
+        <v>274</v>
+      </c>
+      <c r="I80" s="6" t="str">
+        <f>IF(L80&gt;0," || obj_meas_type == "&amp;B80,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x4E</v>
+      </c>
+      <c r="J80" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K80" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <f>IFERROR(ABS(LOG10(E80)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M80" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="N80" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x64,	 // 0x4E | volume | uint32 (4 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 4E87562A01</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <f t="shared" si="9"/>
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>285</v>
+      </c>
+      <c r="C81" t="s">
+        <v>286</v>
+      </c>
+      <c r="D81" t="s">
+        <v>241</v>
+      </c>
+      <c r="E81">
+        <v>1E-3</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="G81">
+        <v>19551.879000000001</v>
+      </c>
+      <c r="H81" t="s">
+        <v>274</v>
+      </c>
+      <c r="I81" s="6" t="str">
+        <f>IF(L81&gt;0," || obj_meas_type == "&amp;B81,"")</f>
+        <v xml:space="preserve"> || obj_meas_type == 0x4F</v>
+      </c>
+      <c r="J81" s="6">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="K81" s="6">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L81">
+        <f>IFERROR(ABS(LOG10(E81)),0)</f>
+        <v>3</v>
+      </c>
+      <c r="M81" s="6" t="str">
+        <f t="shared" si="7"/>
+        <v>64</v>
+      </c>
+      <c r="N81" s="6" t="str">
+        <f t="shared" si="8"/>
+        <v>0x64,	 // 0x4F | water | uint32 (4 bytes) | datatype: 0 | factor_exp10: 0.001 | example: 4F87562A01</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F82"/>
+      <c r="G82" s="3"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F83"/>
+      <c r="G83" s="3"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>178</v>
+      </c>
+      <c r="C84" t="s">
+        <v>197</v>
+      </c>
+      <c r="D84" t="s">
+        <v>198</v>
+      </c>
+      <c r="E84" t="s">
+        <v>199</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="G84" t="s">
+        <v>3</v>
+      </c>
+      <c r="H84" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <f t="shared" ref="A85" si="10">HEX2DEC(SUBSTITUTE(B85,"0x",""))</f>
+        <v>58</v>
+      </c>
+      <c r="B85" t="s">
+        <v>152</v>
+      </c>
+      <c r="C85" t="s">
+        <v>153</v>
+      </c>
+      <c r="D85" t="s">
+        <v>150</v>
+      </c>
+      <c r="E85" t="s">
+        <v>154</v>
+      </c>
+      <c r="G85" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" t="s">
+        <v>156</v>
+      </c>
+      <c r="F86"/>
+      <c r="G86" t="s">
+        <v>328</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>158</v>
+      </c>
+      <c r="F87"/>
+      <c r="G87" t="s">
+        <v>329</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D88" t="s">
+        <v>13</v>
+      </c>
+      <c r="E88" t="s">
+        <v>160</v>
+      </c>
+      <c r="F88"/>
+      <c r="G88" t="s">
+        <v>330</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D89" t="s">
+        <v>17</v>
+      </c>
+      <c r="E89" t="s">
+        <v>162</v>
+      </c>
+      <c r="F89"/>
+      <c r="G89" t="s">
+        <v>331</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D90" t="s">
+        <v>21</v>
+      </c>
+      <c r="E90" t="s">
+        <v>164</v>
+      </c>
+      <c r="F90"/>
+      <c r="G90" t="s">
+        <v>332</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D91" t="s">
+        <v>25</v>
+      </c>
+      <c r="E91" t="s">
+        <v>166</v>
+      </c>
+      <c r="F91"/>
+      <c r="G91" t="s">
+        <v>333</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <f t="shared" ref="A92" si="11">HEX2DEC(SUBSTITUTE(B92,"0x",""))</f>
+        <v>60</v>
+      </c>
+      <c r="B92" t="s">
+        <v>168</v>
+      </c>
+      <c r="C92" t="s">
+        <v>169</v>
+      </c>
+      <c r="D92" t="s">
+        <v>150</v>
+      </c>
+      <c r="E92" t="s">
+        <v>154</v>
+      </c>
+      <c r="G92" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D93" t="s">
+        <v>6</v>
+      </c>
+      <c r="E93" t="s">
+        <v>171</v>
+      </c>
+      <c r="F93" t="s">
+        <v>172</v>
+      </c>
+      <c r="G93" t="s">
+        <v>335</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>175</v>
+      </c>
+      <c r="F94" t="s">
+        <v>172</v>
+      </c>
+      <c r="G94" t="s">
+        <v>336</v>
+      </c>
+      <c r="H94" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:I81" xr:uid="{28042196-756D-49C6-ACCE-21EFE4A952B1}"/>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K1:K1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF5A8AC6"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>